<commit_message>
Bug in liq calc fixed
</commit_message>
<xml_diff>
--- a/qa-scenarios/0038-liquidity-provision-order-type.xlsx
+++ b/qa-scenarios/0038-liquidity-provision-order-type.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidsiska/gits/code.vegaprotocol.io/product/qa-scenarios/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C53CA58A-B861-C047-8E87-CC4AD62627F9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C178AF3C-0FFC-FB4E-BFB3-57D38BE5BAF5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" activeTab="1" xr2:uid="{2A80095B-6965-4E4E-A3A4-8340E9E3ADBC}"/>
   </bookViews>
@@ -371,15 +371,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
@@ -413,8 +414,10 @@
     <xf numFmtId="170" fontId="4" fillId="2" borderId="0" xfId="4" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="171" fontId="4" fillId="2" borderId="0" xfId="4" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="171" fontId="4" fillId="3" borderId="0" xfId="4" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="6" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
+    <cellStyle name="Comma" xfId="6" builtinId="3"/>
     <cellStyle name="Comma 2" xfId="3" xr:uid="{5E9238CA-D7BA-C84A-94B8-10CA583097D8}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{08F1C507-6ACD-B94E-89DD-CD7512B2657C}"/>
@@ -919,7 +922,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56542D29-7BB1-F043-9602-AF51A2F34194}">
   <dimension ref="B2:Z193"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2261,7 +2266,7 @@
         <v>30</v>
       </c>
       <c r="C26" s="15">
-        <f>SUM(U3:U33)</f>
+        <f>SUM(U3:U24)</f>
         <v>1</v>
       </c>
       <c r="D26" s="21" t="s">
@@ -2323,7 +2328,7 @@
         <v>29</v>
       </c>
       <c r="C27" s="15">
-        <f>SUM(U26:U177)</f>
+        <f>SUM(U26:U45)</f>
         <v>1</v>
       </c>
       <c r="D27" s="21" t="s">
@@ -4922,7 +4927,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DFD0C1A-219E-FA43-8902-E51572F832C8}">
   <dimension ref="B2:Z193"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4939,7 +4946,9 @@
     <col min="11" max="11" width="20.83203125" style="11" customWidth="1"/>
     <col min="12" max="12" width="12" style="11" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14.6640625" style="11" customWidth="1"/>
-    <col min="14" max="23" width="10.83203125" style="11"/>
+    <col min="14" max="14" width="10.83203125" style="11"/>
+    <col min="15" max="15" width="12.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="23" width="10.83203125" style="11"/>
     <col min="24" max="24" width="14.1640625" style="11" bestFit="1" customWidth="1"/>
     <col min="25" max="16384" width="10.83203125" style="11"/>
   </cols>
@@ -5632,15 +5641,15 @@
       </c>
       <c r="K15" s="15">
         <f t="shared" si="6"/>
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="L15" s="15">
         <f t="shared" si="7"/>
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="M15" s="14">
         <f>L15*$G$25*RiskFactors!$C$24</f>
-        <v>12.602504809322911</v>
+        <v>23.80473130649883</v>
       </c>
       <c r="U15" s="11">
         <f t="shared" si="2"/>
@@ -5648,7 +5657,7 @@
       </c>
       <c r="V15" s="11">
         <f t="shared" si="3"/>
-        <v>7.1428571428571425E-2</v>
+        <v>0.14285714285714285</v>
       </c>
       <c r="X15" s="12">
         <f t="shared" si="4"/>
@@ -5691,15 +5700,15 @@
       </c>
       <c r="K16" s="15">
         <f t="shared" si="6"/>
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="L16" s="15">
         <f t="shared" si="7"/>
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="M16" s="14">
         <f>L16*$G$25*RiskFactors!$C$24</f>
-        <v>12.602504809322911</v>
+        <v>23.80473130649883</v>
       </c>
       <c r="U16" s="11">
         <f t="shared" si="2"/>
@@ -5707,7 +5716,7 @@
       </c>
       <c r="V16" s="11">
         <f t="shared" si="3"/>
-        <v>7.1428571428571425E-2</v>
+        <v>0.14285714285714285</v>
       </c>
       <c r="X16" s="12">
         <f t="shared" si="4"/>
@@ -5743,15 +5752,15 @@
       </c>
       <c r="K17" s="15">
         <f t="shared" si="6"/>
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="L17" s="15">
         <f t="shared" si="7"/>
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="M17" s="14">
         <f>L17*$G$25*RiskFactors!$C$24</f>
-        <v>12.602504809322911</v>
+        <v>23.80473130649883</v>
       </c>
       <c r="U17" s="11">
         <f t="shared" si="2"/>
@@ -5759,7 +5768,7 @@
       </c>
       <c r="V17" s="11">
         <f t="shared" si="3"/>
-        <v>7.1428571428571425E-2</v>
+        <v>0.14285714285714285</v>
       </c>
       <c r="X17" s="12">
         <f t="shared" si="4"/>
@@ -5795,15 +5804,15 @@
       </c>
       <c r="K18" s="15">
         <f t="shared" si="6"/>
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="L18" s="15">
         <f t="shared" si="7"/>
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="M18" s="14">
         <f>L18*$G$25*RiskFactors!$C$24</f>
-        <v>12.602504809322911</v>
+        <v>23.80473130649883</v>
       </c>
       <c r="U18" s="11">
         <f t="shared" si="2"/>
@@ -5811,7 +5820,7 @@
       </c>
       <c r="V18" s="11">
         <f t="shared" si="3"/>
-        <v>7.1428571428571425E-2</v>
+        <v>0.14285714285714285</v>
       </c>
       <c r="X18" s="12">
         <f t="shared" si="4"/>
@@ -5852,15 +5861,15 @@
       </c>
       <c r="K19" s="15">
         <f t="shared" si="6"/>
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="L19" s="15">
         <f t="shared" si="7"/>
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="M19" s="14">
         <f>L19*$G$25*RiskFactors!$C$24</f>
-        <v>12.602504809322911</v>
+        <v>23.80473130649883</v>
       </c>
       <c r="U19" s="11">
         <f t="shared" si="2"/>
@@ -5868,7 +5877,7 @@
       </c>
       <c r="V19" s="11">
         <f t="shared" si="3"/>
-        <v>7.1428571428571425E-2</v>
+        <v>0.14285714285714285</v>
       </c>
       <c r="X19" s="12">
         <f t="shared" si="4"/>
@@ -5913,15 +5922,15 @@
       </c>
       <c r="K20" s="15">
         <f t="shared" si="6"/>
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="L20" s="15">
         <f t="shared" si="7"/>
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="M20" s="14">
         <f>L20*$G$25*RiskFactors!$C$24</f>
-        <v>12.602504809322911</v>
+        <v>23.80473130649883</v>
       </c>
       <c r="U20" s="11">
         <f t="shared" si="2"/>
@@ -5929,7 +5938,7 @@
       </c>
       <c r="V20" s="11">
         <f t="shared" si="3"/>
-        <v>7.1428571428571425E-2</v>
+        <v>0.14285714285714285</v>
       </c>
       <c r="X20" s="12">
         <f t="shared" si="4"/>
@@ -5976,15 +5985,15 @@
       </c>
       <c r="K21" s="15">
         <f t="shared" si="6"/>
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="L21" s="15">
         <f t="shared" si="7"/>
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="M21" s="14">
         <f>L21*$G$25*RiskFactors!$C$24</f>
-        <v>12.602504809322911</v>
+        <v>23.80473130649883</v>
       </c>
       <c r="U21" s="11">
         <f t="shared" si="2"/>
@@ -5992,7 +6001,7 @@
       </c>
       <c r="V21" s="11">
         <f t="shared" si="3"/>
-        <v>7.1428571428571425E-2</v>
+        <v>0.14285714285714285</v>
       </c>
       <c r="X21" s="12">
         <f t="shared" si="4"/>
@@ -6013,7 +6022,7 @@
       </c>
       <c r="C22" s="20">
         <f>SUMPRODUCT(G3:G33,H3:H33,I3:I33)</f>
-        <v>2995.7039780400232</v>
+        <v>2995.7615933653738</v>
       </c>
       <c r="D22" s="15" t="str">
         <f>$C$15&amp;"-siskas"</f>
@@ -6032,7 +6041,7 @@
         <v>0.49928345544959374</v>
       </c>
       <c r="I22" s="17">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="J22" s="16">
         <v>0</v>
@@ -6043,12 +6052,13 @@
       </c>
       <c r="L22" s="15">
         <f t="shared" si="7"/>
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="M22" s="14">
         <f>L22*$G$25*RiskFactors!$C$24</f>
-        <v>70.013915607349503</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="O22" s="33"/>
       <c r="U22" s="11">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -6095,7 +6105,7 @@
         <v>0.49929309960112933</v>
       </c>
       <c r="I23" s="17">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="J23" s="16">
         <v>0</v>
@@ -6106,11 +6116,11 @@
       </c>
       <c r="L23" s="15">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M23" s="14">
         <f>L23*$G$25*RiskFactors!$C$24</f>
-        <v>0</v>
+        <v>70.013915607349503</v>
       </c>
       <c r="U23" s="11">
         <f t="shared" si="2"/>
@@ -6139,7 +6149,7 @@
       </c>
       <c r="C24" s="20">
         <f>MAX(C21-C22,0)</f>
-        <v>7004.2960219599772</v>
+        <v>7004.2384066346258</v>
       </c>
       <c r="D24" s="15" t="str">
         <f>$C$15&amp;"-siskas"</f>
@@ -6264,8 +6274,8 @@
         <v>30</v>
       </c>
       <c r="C26" s="15">
-        <f>SUM(U3:U33)</f>
-        <v>14</v>
+        <f>SUM(U4:U24)</f>
+        <v>7</v>
       </c>
       <c r="D26" s="21" t="s">
         <v>28</v>
@@ -6326,7 +6336,7 @@
         <v>29</v>
       </c>
       <c r="C27" s="15">
-        <f>SUM(U26:U177)</f>
+        <f>SUM(U26:U45)</f>
         <v>9</v>
       </c>
       <c r="D27" s="21" t="s">
@@ -6389,7 +6399,7 @@
       </c>
       <c r="C28" s="20">
         <f>SUMPRODUCT(G3:G33,H3:H33,L3:L33)</f>
-        <v>14760.208623578588</v>
+        <v>18115.196577620609</v>
       </c>
       <c r="D28" s="19" t="s">
         <v>25</v>
@@ -6622,7 +6632,7 @@
       </c>
       <c r="C32" s="18">
         <f>SUM(M3:M33)</f>
-        <v>342.49509212758193</v>
+        <v>420.91067760781334</v>
       </c>
       <c r="D32" s="15" t="str">
         <f>C15</f>
@@ -6857,7 +6867,7 @@
       </c>
       <c r="C36" s="14">
         <f>C20+SUM(C32:C33)</f>
-        <v>11756.438635486365</v>
+        <v>11834.854220966597</v>
       </c>
       <c r="D36" s="15" t="str">
         <f>C15</f>
@@ -8459,7 +8469,7 @@
       </c>
       <c r="L112" s="15">
         <f t="shared" si="24"/>
-        <v>176</v>
+        <v>184</v>
       </c>
     </row>
     <row r="113" spans="5:12" x14ac:dyDescent="0.2">
@@ -8473,7 +8483,7 @@
       </c>
       <c r="L113" s="15">
         <f t="shared" si="24"/>
-        <v>59</v>
+        <v>67</v>
       </c>
     </row>
     <row r="114" spans="5:12" x14ac:dyDescent="0.2">
@@ -8487,7 +8497,7 @@
       </c>
       <c r="L114" s="15">
         <f t="shared" si="24"/>
-        <v>59</v>
+        <v>67</v>
       </c>
     </row>
     <row r="115" spans="5:12" x14ac:dyDescent="0.2">
@@ -8501,7 +8511,7 @@
       </c>
       <c r="L115" s="15">
         <f t="shared" si="24"/>
-        <v>59</v>
+        <v>67</v>
       </c>
     </row>
     <row r="116" spans="5:12" x14ac:dyDescent="0.2">
@@ -8515,7 +8525,7 @@
       </c>
       <c r="L116" s="15">
         <f t="shared" si="24"/>
-        <v>59</v>
+        <v>67</v>
       </c>
     </row>
     <row r="117" spans="5:12" x14ac:dyDescent="0.2">
@@ -8529,7 +8539,7 @@
       </c>
       <c r="L117" s="15">
         <f t="shared" si="24"/>
-        <v>59</v>
+        <v>67</v>
       </c>
     </row>
     <row r="118" spans="5:12" x14ac:dyDescent="0.2">
@@ -8543,7 +8553,7 @@
       </c>
       <c r="L118" s="15">
         <f t="shared" si="24"/>
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="119" spans="5:12" x14ac:dyDescent="0.2">
@@ -8557,7 +8567,7 @@
       </c>
       <c r="L119" s="15">
         <f t="shared" si="24"/>
-        <v>50</v>
+        <v>0</v>
       </c>
     </row>
     <row r="120" spans="5:12" x14ac:dyDescent="0.2">
@@ -8571,7 +8581,7 @@
       </c>
       <c r="L120" s="15">
         <f t="shared" si="24"/>
-        <v>0</v>
+        <v>50</v>
       </c>
     </row>
     <row r="121" spans="5:12" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update the values to reflec best bid best ask change when using prob of trading
</commit_message>
<xml_diff>
--- a/qa-scenarios/0038-liquidity-provision-order-type.xlsx
+++ b/qa-scenarios/0038-liquidity-provision-order-type.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidsiska/gits/code.vegaprotocol.io/product/qa-scenarios/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C178AF3C-0FFC-FB4E-BFB3-57D38BE5BAF5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37ABD0FC-1D85-BB42-BE3B-76F07C6D4485}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" activeTab="1" xr2:uid="{2A80095B-6965-4E4E-A3A4-8340E9E3ADBC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="76">
   <si>
     <t>Long</t>
   </si>
@@ -252,6 +252,18 @@
   </si>
   <si>
     <t>Total book volume</t>
+  </si>
+  <si>
+    <t>Best ask</t>
+  </si>
+  <si>
+    <t>Best bid</t>
+  </si>
+  <si>
+    <t>Current best ask</t>
+  </si>
+  <si>
+    <t>Current best bid</t>
   </si>
 </sst>
 </file>
@@ -772,14 +784,14 @@
       </c>
       <c r="C5" s="9">
         <f>'Step 1'!C10</f>
-        <v>1.9012852688417371E-6</v>
+        <v>1.1407711613050422E-4</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E5" s="1">
         <f>C5*365.25*24*60</f>
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>15</v>
@@ -791,7 +803,7 @@
       </c>
       <c r="C6" s="8">
         <f>'Step 1'!C8</f>
-        <v>2.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.2">
@@ -808,7 +820,7 @@
       </c>
       <c r="C9" s="3">
         <f>SQRT(C5)*C6</f>
-        <v>3.4471775310042935E-3</v>
+        <v>2.1361377870400048E-2</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.2">
@@ -817,7 +829,7 @@
       </c>
       <c r="C10" s="3">
         <f>C7-0.5*C6*C6*C5</f>
-        <v>-5.9415164651304284E-6</v>
+        <v>-2.2815423226100844E-4</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.2">
@@ -844,7 +856,7 @@
       </c>
       <c r="C17" s="3">
         <f>(1/C4)*EXP(C10+C9*C9*0.5)* ( 1 - _xlfn.NORM.S.DIST(C12-C9,TRUE))</f>
-        <v>1.0116689762104114</v>
+        <v>1.0743470111445053</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.2">
@@ -853,7 +865,7 @@
       </c>
       <c r="C18" s="3">
         <f>-(1/C4)*EXP(C10*C9*C9*0.5) * _xlfn.NORM.S.DIST(C11-C9,TRUE)</f>
-        <v>-0.98845466859009623</v>
+        <v>-0.93040205381372454</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.2">
@@ -868,7 +880,7 @@
       </c>
       <c r="C24" s="6">
         <f>C17-1</f>
-        <v>1.1668976210411408E-2</v>
+        <v>7.4347011144505259E-2</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.2">
@@ -877,7 +889,7 @@
       </c>
       <c r="C25" s="3">
         <f>C18+1</f>
-        <v>1.154533140990377E-2</v>
+        <v>6.9597946186275461E-2</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.2">
@@ -901,7 +913,7 @@
       </c>
       <c r="C29" s="2">
         <f>1/C24</f>
-        <v>85.697320996144484</v>
+        <v>13.450439830813652</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.2">
@@ -910,7 +922,7 @@
       </c>
       <c r="C30" s="2">
         <f>1/C25</f>
-        <v>86.615097002948218</v>
+        <v>14.36824008173387</v>
       </c>
     </row>
   </sheetData>
@@ -922,8 +934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56542D29-7BB1-F043-9602-AF51A2F34194}">
   <dimension ref="B2:Z193"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -932,14 +944,14 @@
     <col min="2" max="2" width="28" style="11" customWidth="1"/>
     <col min="3" max="3" width="18.6640625" style="11" customWidth="1"/>
     <col min="4" max="4" width="10.83203125" style="11"/>
-    <col min="5" max="5" width="8.33203125" style="11" customWidth="1"/>
+    <col min="5" max="5" width="14" style="11" customWidth="1"/>
     <col min="6" max="6" width="22.83203125" style="11" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" style="11"/>
+    <col min="7" max="7" width="10.83203125" style="11" customWidth="1"/>
     <col min="8" max="8" width="11.83203125" style="11" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="24.1640625" style="11" customWidth="1"/>
     <col min="10" max="10" width="10.83203125" style="11"/>
     <col min="11" max="11" width="26.1640625" style="11" customWidth="1"/>
-    <col min="12" max="12" width="16.33203125" style="11" customWidth="1"/>
+    <col min="12" max="12" width="22.83203125" style="11" customWidth="1"/>
     <col min="13" max="13" width="14.6640625" style="11" customWidth="1"/>
     <col min="14" max="23" width="10.83203125" style="11"/>
     <col min="24" max="24" width="14.1640625" style="11" bestFit="1" customWidth="1"/>
@@ -1008,8 +1020,8 @@
         <v>21</v>
       </c>
       <c r="G4" s="30">
-        <f t="shared" ref="G4:G24" si="1">G5+$C$14</f>
-        <v>120.00021000000007</v>
+        <f t="shared" ref="G4:G24" si="1">G5+$C$15</f>
+        <v>123.09999999999988</v>
       </c>
       <c r="U4" s="11">
         <f t="shared" ref="U4:U24" si="2">IF(H4&lt;0.0000000001,0,J4)</f>
@@ -1020,8 +1032,8 @@
         <v>0</v>
       </c>
       <c r="X4" s="12">
-        <f t="shared" ref="X4:X45" si="4">(LN(G4/$C$13)-($C$7-0.5*$C$8*$C$8)*$C$10)/($C$8*SQRT($C$10))</f>
-        <v>2.2312500198120172E-3</v>
+        <f t="shared" ref="X4:X25" si="4">(LN(G4/$C$13)-($C$7-0.5*$C$8*$C$8)*$C$10)/($C$8*SQRT($C$10))</f>
+        <v>0.81617590081047908</v>
       </c>
       <c r="Y4" s="12"/>
       <c r="Z4" s="12"/>
@@ -1033,11 +1045,11 @@
       </c>
       <c r="G5" s="30">
         <f t="shared" si="1"/>
-        <v>120.00020000000006</v>
+        <v>122.99999999999989</v>
       </c>
       <c r="H5" s="31">
         <f t="shared" ref="H5:H24" si="5">1-_xlfn.NORM.DIST(X5,0,1,TRUE)</f>
-        <v>0.49911950490425294</v>
+        <v>0.21824570569335955</v>
       </c>
       <c r="I5" s="17">
         <v>0</v>
@@ -1067,15 +1079,15 @@
       </c>
       <c r="X5" s="12">
         <f t="shared" si="4"/>
-        <v>2.207075694517017E-3</v>
+        <v>0.77813164060775064</v>
       </c>
       <c r="Y5" s="12">
-        <f t="shared" ref="Y5:Y45" si="8">(LN(G4/$C$13)-($C$7-0.5*$C$8*$C$8)*$C$10)/($C$8*SQRT($C$10))</f>
-        <v>2.2312500198120172E-3</v>
+        <f t="shared" ref="Y5:Y25" si="8">(LN(G4/$C$13)-($C$7-0.5*$C$8*$C$8)*$C$10)/($C$8*SQRT($C$10))</f>
+        <v>0.81617590081047908</v>
       </c>
       <c r="Z5" s="12">
-        <f t="shared" ref="Z5:Z45" si="9">_xlfn.NORM.DIST(Y5,0,1,TRUE)-_xlfn.NORM.DIST(X5,0,1,TRUE)</f>
-        <v>9.6441367127830802E-6</v>
+        <f t="shared" ref="Z5:Z25" si="9">_xlfn.NORM.DIST(Y5,0,1,TRUE)-_xlfn.NORM.DIST(X5,0,1,TRUE)</f>
+        <v>1.104593667385112E-2</v>
       </c>
     </row>
     <row r="6" spans="2:26" x14ac:dyDescent="0.2">
@@ -1090,11 +1102,11 @@
       </c>
       <c r="G6" s="30">
         <f t="shared" si="1"/>
-        <v>120.00019000000006</v>
+        <v>122.89999999999989</v>
       </c>
       <c r="H6" s="31">
         <f t="shared" si="5"/>
-        <v>0.49912914904228423</v>
+        <v>0.22963287498043239</v>
       </c>
       <c r="I6" s="17">
         <v>0</v>
@@ -1124,15 +1136,15 @@
       </c>
       <c r="X6" s="12">
         <f t="shared" si="4"/>
-        <v>2.1829013672074928E-3</v>
+        <v>0.74005643753036121</v>
       </c>
       <c r="Y6" s="12">
         <f t="shared" si="8"/>
-        <v>2.207075694517017E-3</v>
+        <v>0.77813164060775064</v>
       </c>
       <c r="Z6" s="12">
         <f t="shared" si="9"/>
-        <v>9.6441380312839442E-6</v>
+        <v>1.138716928707284E-2</v>
       </c>
     </row>
     <row r="7" spans="2:26" x14ac:dyDescent="0.2">
@@ -1149,11 +1161,11 @@
       </c>
       <c r="G7" s="30">
         <f t="shared" si="1"/>
-        <v>120.00018000000006</v>
+        <v>122.7999999999999</v>
       </c>
       <c r="H7" s="31">
         <f t="shared" si="5"/>
-        <v>0.4991387931816279</v>
+        <v>0.24135509760665552</v>
       </c>
       <c r="I7" s="17">
         <v>0</v>
@@ -1183,15 +1195,15 @@
       </c>
       <c r="X7" s="12">
         <f t="shared" si="4"/>
-        <v>2.1587270378834447E-3</v>
+        <v>0.70195024120325233</v>
       </c>
       <c r="Y7" s="12">
         <f t="shared" si="8"/>
-        <v>2.1829013672074928E-3</v>
+        <v>0.74005643753036121</v>
       </c>
       <c r="Z7" s="12">
         <f t="shared" si="9"/>
-        <v>9.6441393436785816E-6</v>
+        <v>1.1722222626223133E-2</v>
       </c>
     </row>
     <row r="8" spans="2:26" x14ac:dyDescent="0.2">
@@ -1199,7 +1211,7 @@
         <v>14</v>
       </c>
       <c r="C8" s="28">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="D8" s="15"/>
       <c r="F8" s="15">
@@ -1208,11 +1220,11 @@
       </c>
       <c r="G8" s="30">
         <f t="shared" si="1"/>
-        <v>120.00017000000005</v>
+        <v>122.6999999999999</v>
       </c>
       <c r="H8" s="31">
         <f t="shared" si="5"/>
-        <v>0.49914843732227865</v>
+        <v>0.25340500175444125</v>
       </c>
       <c r="I8" s="17">
         <v>0</v>
@@ -1242,15 +1254,15 @@
       </c>
       <c r="X8" s="12">
         <f t="shared" si="4"/>
-        <v>2.1345527065448717E-3</v>
+        <v>0.66381300112824893</v>
       </c>
       <c r="Y8" s="12">
         <f t="shared" si="8"/>
-        <v>2.1587270378834447E-3</v>
+        <v>0.70195024120325233</v>
       </c>
       <c r="Z8" s="12">
         <f t="shared" si="9"/>
-        <v>9.6441406507441485E-6</v>
+        <v>1.2049904147785728E-2</v>
       </c>
     </row>
     <row r="9" spans="2:26" x14ac:dyDescent="0.2">
@@ -1258,7 +1270,7 @@
         <v>17</v>
       </c>
       <c r="C9" s="16">
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="D9" s="15" t="s">
         <v>49</v>
@@ -1269,11 +1281,11 @@
       </c>
       <c r="G9" s="30">
         <f t="shared" si="1"/>
-        <v>120.00016000000005</v>
+        <v>122.59999999999991</v>
       </c>
       <c r="H9" s="31">
         <f t="shared" si="5"/>
-        <v>0.49915808146423069</v>
+        <v>0.26577401723373129</v>
       </c>
       <c r="I9" s="17">
         <v>0</v>
@@ -1303,15 +1315,15 @@
       </c>
       <c r="X9" s="12">
         <f t="shared" si="4"/>
-        <v>2.1103783731917739E-3</v>
+        <v>0.62564466668365837</v>
       </c>
       <c r="Y9" s="12">
         <f t="shared" si="8"/>
-        <v>2.1345527065448717E-3</v>
+        <v>0.66381300112824893</v>
       </c>
       <c r="Z9" s="12">
         <f t="shared" si="9"/>
-        <v>9.6441419520365557E-6</v>
+        <v>1.2369015479290035E-2</v>
       </c>
     </row>
     <row r="10" spans="2:26" x14ac:dyDescent="0.2">
@@ -1320,7 +1332,7 @@
       </c>
       <c r="C10" s="27">
         <f>C9/60/24/365.25</f>
-        <v>1.9012852688417371E-6</v>
+        <v>1.1407711613050422E-4</v>
       </c>
       <c r="D10" s="15" t="s">
         <v>48</v>
@@ -1331,11 +1343,11 @@
       </c>
       <c r="G10" s="30">
         <f t="shared" si="1"/>
-        <v>120.00015000000005</v>
+        <v>122.49999999999991</v>
       </c>
       <c r="H10" s="31">
         <f t="shared" si="5"/>
-        <v>0.49916772560747846</v>
+        <v>0.27845237659158517</v>
       </c>
       <c r="I10" s="17">
         <v>0</v>
@@ -1365,15 +1377,15 @@
       </c>
       <c r="X10" s="12">
         <f t="shared" si="4"/>
-        <v>2.0862040378241513E-3</v>
+        <v>0.58744518712387717</v>
       </c>
       <c r="Y10" s="12">
         <f t="shared" si="8"/>
-        <v>2.1103783731917739E-3</v>
+        <v>0.62564466668365837</v>
       </c>
       <c r="Z10" s="12">
         <f t="shared" si="9"/>
-        <v>9.6441432477778477E-6</v>
+        <v>1.2678359357853886E-2</v>
       </c>
     </row>
     <row r="11" spans="2:26" x14ac:dyDescent="0.2">
@@ -1383,11 +1395,11 @@
       </c>
       <c r="G11" s="30">
         <f t="shared" si="1"/>
-        <v>120.00014000000004</v>
+        <v>122.39999999999992</v>
       </c>
       <c r="H11" s="31">
         <f t="shared" si="5"/>
-        <v>0.49917736975201632</v>
+        <v>0.29142912338445615</v>
       </c>
       <c r="I11" s="17">
         <v>0</v>
@@ -1417,15 +1429,15 @@
       </c>
       <c r="X11" s="12">
         <f t="shared" si="4"/>
-        <v>2.062029700442003E-3</v>
+        <v>0.54921451157894574</v>
       </c>
       <c r="Y11" s="12">
         <f t="shared" si="8"/>
-        <v>2.0862040378241513E-3</v>
+        <v>0.58744518712387717</v>
       </c>
       <c r="Z11" s="12">
         <f t="shared" si="9"/>
-        <v>9.6441445378570023E-6</v>
+        <v>1.2976746792870975E-2</v>
       </c>
     </row>
     <row r="12" spans="2:26" x14ac:dyDescent="0.2">
@@ -1440,11 +1452,11 @@
       </c>
       <c r="G12" s="30">
         <f t="shared" si="1"/>
-        <v>120.00013000000004</v>
+        <v>122.29999999999993</v>
       </c>
       <c r="H12" s="31">
         <f t="shared" si="5"/>
-        <v>0.49918701389783848</v>
+        <v>0.30469212778082255</v>
       </c>
       <c r="I12" s="17">
         <v>0</v>
@@ -1474,26 +1486,26 @@
       </c>
       <c r="X12" s="12">
         <f t="shared" si="4"/>
-        <v>2.0378553610453289E-3</v>
+        <v>0.51095258905420249</v>
       </c>
       <c r="Y12" s="12">
         <f t="shared" si="8"/>
-        <v>2.062029700442003E-3</v>
+        <v>0.54921451157894574</v>
       </c>
       <c r="Z12" s="12">
         <f t="shared" si="9"/>
-        <v>9.6441458221629972E-6</v>
+        <v>1.3263004396366407E-2</v>
       </c>
     </row>
     <row r="13" spans="2:26" x14ac:dyDescent="0.2">
-      <c r="B13" s="15" t="s">
-        <v>63</v>
+      <c r="B13" s="21" t="s">
+        <v>74</v>
       </c>
       <c r="C13" s="16">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D13" s="21" t="str">
-        <f>C15&amp;" to "&amp;C16</f>
+        <f>C16&amp;" to "&amp;C17</f>
         <v>USD to AAPL</v>
       </c>
       <c r="F13" s="15">
@@ -1502,11 +1514,11 @@
       </c>
       <c r="G13" s="30">
         <f t="shared" si="1"/>
-        <v>120.00012000000004</v>
+        <v>122.19999999999993</v>
       </c>
       <c r="H13" s="31">
         <f t="shared" si="5"/>
-        <v>0.49919665804493951</v>
+        <v>0.31822810960184511</v>
       </c>
       <c r="I13" s="17">
         <v>0</v>
@@ -1536,36 +1548,39 @@
       </c>
       <c r="X13" s="12">
         <f t="shared" si="4"/>
-        <v>2.0136810196341288E-3</v>
+        <v>0.47265936842983552</v>
       </c>
       <c r="Y13" s="12">
         <f t="shared" si="8"/>
-        <v>2.0378553610453289E-3</v>
+        <v>0.51095258905420249</v>
       </c>
       <c r="Z13" s="12">
         <f t="shared" si="9"/>
-        <v>9.6441471010288993E-6</v>
+        <v>1.3535981821022558E-2</v>
       </c>
     </row>
     <row r="14" spans="2:26" x14ac:dyDescent="0.2">
-      <c r="B14" s="15" t="s">
-        <v>46</v>
+      <c r="B14" s="21" t="s">
+        <v>75</v>
       </c>
       <c r="C14" s="16">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="D14" s="15"/>
+        <v>119</v>
+      </c>
+      <c r="D14" s="21" t="str">
+        <f>C17&amp;" to "&amp;C18</f>
+        <v xml:space="preserve">AAPL to </v>
+      </c>
       <c r="F14" s="15">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="G14" s="30">
         <f t="shared" si="1"/>
-        <v>120.00011000000003</v>
+        <v>122.09999999999994</v>
       </c>
       <c r="H14" s="31">
         <f t="shared" si="5"/>
-        <v>0.49920630219331374</v>
+        <v>0.3320226688443878</v>
       </c>
       <c r="I14" s="17">
         <v>0</v>
@@ -1595,23 +1610,23 @@
       </c>
       <c r="X14" s="12">
         <f t="shared" si="4"/>
-        <v>1.9895066762084016E-3</v>
+        <v>0.4343347984604829</v>
       </c>
       <c r="Y14" s="12">
         <f t="shared" si="8"/>
-        <v>2.0136810196341288E-3</v>
+        <v>0.47265936842983552</v>
       </c>
       <c r="Z14" s="12">
         <f t="shared" si="9"/>
-        <v>9.6441483742326639E-6</v>
+        <v>1.3794559242542692E-2</v>
       </c>
     </row>
     <row r="15" spans="2:26" x14ac:dyDescent="0.2">
-      <c r="B15" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="C15" s="26" t="s">
-        <v>41</v>
+      <c r="B15" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="16">
+        <v>0.1</v>
       </c>
       <c r="D15" s="15"/>
       <c r="F15" s="15">
@@ -1620,11 +1635,11 @@
       </c>
       <c r="G15" s="30">
         <f t="shared" si="1"/>
-        <v>120.00010000000003</v>
+        <v>121.99999999999994</v>
       </c>
       <c r="H15" s="31">
         <f t="shared" si="5"/>
-        <v>0.4992159463429553</v>
+        <v>0.34606032366512329</v>
       </c>
       <c r="I15" s="17">
         <v>0</v>
@@ -1634,15 +1649,15 @@
       </c>
       <c r="K15" s="15">
         <f t="shared" si="6"/>
-        <v>167</v>
+        <v>119</v>
       </c>
       <c r="L15" s="15">
         <f t="shared" si="7"/>
-        <v>167</v>
+        <v>119</v>
       </c>
       <c r="M15" s="14">
         <f>L15*$G$25*RiskFactors!$C$24</f>
-        <v>233.84628325664463</v>
+        <v>1070.5226134697311</v>
       </c>
       <c r="U15" s="11">
         <f t="shared" si="2"/>
@@ -1650,27 +1665,27 @@
       </c>
       <c r="V15" s="11">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="X15" s="12">
         <f t="shared" si="4"/>
-        <v>1.9653323307681479E-3</v>
+        <v>0.39597882777482091</v>
       </c>
       <c r="Y15" s="12">
         <f t="shared" si="8"/>
-        <v>1.9895066762084016E-3</v>
+        <v>0.4343347984604829</v>
       </c>
       <c r="Z15" s="12">
         <f t="shared" si="9"/>
-        <v>9.6441496415522465E-6</v>
+        <v>1.403765482073549E-2</v>
       </c>
     </row>
     <row r="16" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B16" s="21" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C16" s="26" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="D16" s="15"/>
       <c r="F16" s="15">
@@ -1679,11 +1694,11 @@
       </c>
       <c r="G16" s="30">
         <f t="shared" si="1"/>
-        <v>120.00009000000003</v>
+        <v>121.89999999999995</v>
       </c>
       <c r="H16" s="31">
         <f t="shared" si="5"/>
-        <v>0.49922559049385895</v>
+        <v>0.36032455573699063</v>
       </c>
       <c r="I16" s="17">
         <v>0</v>
@@ -1713,29 +1728,36 @@
       </c>
       <c r="X16" s="12">
         <f t="shared" si="4"/>
-        <v>1.9411579833133671E-3</v>
+        <v>0.35759140487515118</v>
       </c>
       <c r="Y16" s="12">
         <f t="shared" si="8"/>
-        <v>1.9653323307681479E-3</v>
+        <v>0.39597882777482091</v>
       </c>
       <c r="Z16" s="12">
         <f t="shared" si="9"/>
-        <v>9.6441509036537809E-6</v>
+        <v>1.4264232071867333E-2</v>
       </c>
     </row>
     <row r="17" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B17" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" s="15"/>
       <c r="F17" s="15">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="G17" s="30">
         <f t="shared" si="1"/>
-        <v>120.00008000000003</v>
+        <v>121.79999999999995</v>
       </c>
       <c r="H17" s="31">
         <f t="shared" si="5"/>
-        <v>0.49923523464601871</v>
+        <v>0.3747978628208396</v>
       </c>
       <c r="I17" s="17">
         <v>0</v>
@@ -1765,15 +1787,15 @@
       </c>
       <c r="X17" s="12">
         <f t="shared" si="4"/>
-        <v>1.9169836338440588E-3</v>
+        <v>0.31917247813698574</v>
       </c>
       <c r="Y17" s="12">
         <f t="shared" si="8"/>
-        <v>1.9411579833133671E-3</v>
+        <v>0.35759140487515118</v>
       </c>
       <c r="Z17" s="12">
         <f t="shared" si="9"/>
-        <v>9.644152159760111E-6</v>
+        <v>1.4473307083848974E-2</v>
       </c>
     </row>
     <row r="18" spans="2:26" x14ac:dyDescent="0.2">
@@ -1783,11 +1805,11 @@
       </c>
       <c r="G18" s="30">
         <f t="shared" si="1"/>
-        <v>120.00007000000002</v>
+        <v>121.69999999999996</v>
       </c>
       <c r="H18" s="31">
         <f t="shared" si="5"/>
-        <v>0.49924487879945478</v>
+        <v>0.38946181832644611</v>
       </c>
       <c r="I18" s="17">
         <v>0</v>
@@ -1817,15 +1839,15 @@
       </c>
       <c r="X18" s="12">
         <f t="shared" si="4"/>
-        <v>1.892809282295809E-3</v>
+        <v>0.2807219958086305</v>
       </c>
       <c r="Y18" s="12">
         <f t="shared" si="8"/>
-        <v>1.9169836338440588E-3</v>
+        <v>0.31917247813698574</v>
       </c>
       <c r="Z18" s="12">
         <f t="shared" si="9"/>
-        <v>9.6441534360725001E-6</v>
+        <v>1.4663955505606507E-2</v>
       </c>
     </row>
     <row r="19" spans="2:26" x14ac:dyDescent="0.2">
@@ -1840,11 +1862,11 @@
       </c>
       <c r="G19" s="30">
         <f t="shared" si="1"/>
-        <v>120.00006000000002</v>
+        <v>121.59999999999997</v>
       </c>
       <c r="H19" s="31">
         <f t="shared" si="5"/>
-        <v>0.4992545229541101</v>
+        <v>0.40429713756904351</v>
       </c>
       <c r="I19" s="17">
         <v>0</v>
@@ -1874,15 +1896,15 @@
       </c>
       <c r="X19" s="12">
         <f t="shared" si="4"/>
-        <v>1.8686349287974446E-3</v>
+        <v>0.24223990601076686</v>
       </c>
       <c r="Y19" s="12">
         <f t="shared" si="8"/>
-        <v>1.892809282295809E-3</v>
+        <v>0.2807219958086305</v>
       </c>
       <c r="Z19" s="12">
         <f t="shared" si="9"/>
-        <v>9.6441546553194257E-6</v>
+        <v>1.48353192425974E-2</v>
       </c>
     </row>
     <row r="20" spans="2:26" x14ac:dyDescent="0.2">
@@ -1901,11 +1923,11 @@
       </c>
       <c r="G20" s="30">
         <f t="shared" si="1"/>
-        <v>120.00005000000002</v>
+        <v>121.49999999999997</v>
       </c>
       <c r="H20" s="31">
         <f t="shared" si="5"/>
-        <v>0.49926416711000488</v>
+        <v>0.41928375036089971</v>
       </c>
       <c r="I20" s="17">
         <v>0</v>
@@ -1935,15 +1957,15 @@
       </c>
       <c r="X20" s="12">
         <f t="shared" si="4"/>
-        <v>1.8444605732845516E-3</v>
+        <v>0.20372615673604219</v>
       </c>
       <c r="Y20" s="12">
         <f t="shared" si="8"/>
-        <v>1.8686349287974446E-3</v>
+        <v>0.24223990601076686</v>
       </c>
       <c r="Z20" s="12">
         <f t="shared" si="9"/>
-        <v>9.6441558947724104E-6</v>
+        <v>1.4986612791856202E-2</v>
       </c>
     </row>
     <row r="21" spans="2:26" x14ac:dyDescent="0.2">
@@ -1955,7 +1977,7 @@
         <v>10000</v>
       </c>
       <c r="D21" s="15" t="str">
-        <f>$C$15&amp;"-siskas"</f>
+        <f>$C$16&amp;"-siskas"</f>
         <v>USD-siskas</v>
       </c>
       <c r="F21" s="15">
@@ -1964,49 +1986,49 @@
       </c>
       <c r="G21" s="30">
         <f t="shared" si="1"/>
-        <v>120.00004000000001</v>
+        <v>121.39999999999998</v>
       </c>
       <c r="H21" s="31">
         <f t="shared" si="5"/>
-        <v>0.49927381126713333</v>
+        <v>0.43440087951315898</v>
       </c>
       <c r="I21" s="17">
         <v>0</v>
       </c>
       <c r="J21" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K21" s="15">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>95</v>
       </c>
       <c r="L21" s="15">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>95</v>
       </c>
       <c r="M21" s="14">
         <f>L21*$G$25*RiskFactors!$C$24</f>
-        <v>0</v>
+        <v>854.61889310608797</v>
       </c>
       <c r="U21" s="11">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V21" s="11">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="X21" s="12">
         <f t="shared" si="4"/>
-        <v>1.8202862157571296E-3</v>
+        <v>0.1651806958486067</v>
       </c>
       <c r="Y21" s="12">
         <f t="shared" si="8"/>
-        <v>1.8444605732845516E-3</v>
+        <v>0.20372615673604219</v>
       </c>
       <c r="Z21" s="12">
         <f t="shared" si="9"/>
-        <v>9.6441571284522354E-6</v>
+        <v>1.5117129152259268E-2</v>
       </c>
     </row>
     <row r="22" spans="2:26" x14ac:dyDescent="0.2">
@@ -2014,11 +2036,11 @@
         <v>39</v>
       </c>
       <c r="C22" s="20">
-        <f>SUMPRODUCT(G3:G33,H3:H33,I3:I33)</f>
+        <f>SUMPRODUCT(G3:G34,H3:H34,I3:I34)</f>
         <v>0</v>
       </c>
       <c r="D22" s="15" t="str">
-        <f>$C$15&amp;"-siskas"</f>
+        <f>$C$16&amp;"-siskas"</f>
         <v>USD-siskas</v>
       </c>
       <c r="F22" s="15">
@@ -2027,11 +2049,11 @@
       </c>
       <c r="G22" s="30">
         <f t="shared" si="1"/>
-        <v>120.00003000000001</v>
+        <v>121.29999999999998</v>
       </c>
       <c r="H22" s="31">
         <f t="shared" si="5"/>
-        <v>0.49928345542548969</v>
+        <v>0.4496271247618342</v>
       </c>
       <c r="I22" s="17">
         <v>0</v>
@@ -2061,15 +2083,15 @@
       </c>
       <c r="X22" s="12">
         <f t="shared" si="4"/>
-        <v>1.7961118562151786E-3</v>
+        <v>0.126603471083752</v>
       </c>
       <c r="Y22" s="12">
         <f t="shared" si="8"/>
-        <v>1.8202862157571296E-3</v>
+        <v>0.1651806958486067</v>
       </c>
       <c r="Z22" s="12">
         <f t="shared" si="9"/>
-        <v>9.6441583563589006E-6</v>
+        <v>1.5226245248675219E-2</v>
       </c>
     </row>
     <row r="23" spans="2:26" x14ac:dyDescent="0.2">
@@ -2077,11 +2099,11 @@
         <v>38</v>
       </c>
       <c r="C23" s="20">
-        <f>SUMPRODUCT(G26:G177,H26:H177,I26:I177)</f>
+        <f>SUMPRODUCT(G27:G177,H27:H177,I27:I177)</f>
         <v>0</v>
       </c>
       <c r="D23" s="15" t="str">
-        <f>$C$15&amp;"-siskas"</f>
+        <f>$C$16&amp;"-siskas"</f>
         <v>USD-siskas</v>
       </c>
       <c r="F23" s="15">
@@ -2090,11 +2112,11 @@
       </c>
       <c r="G23" s="30">
         <f t="shared" si="1"/>
-        <v>120.00002000000001</v>
+        <v>121.19999999999999</v>
       </c>
       <c r="H23" s="31">
         <f t="shared" si="5"/>
-        <v>0.49929309958506862</v>
+        <v>0.46494055157462355</v>
       </c>
       <c r="I23" s="17">
         <v>0</v>
@@ -2124,15 +2146,15 @@
       </c>
       <c r="X23" s="12">
         <f t="shared" si="4"/>
-        <v>1.771937494658698E-3</v>
+        <v>8.7994430047444575E-2</v>
       </c>
       <c r="Y23" s="12">
         <f t="shared" si="8"/>
-        <v>1.7961118562151786E-3</v>
+        <v>0.126603471083752</v>
       </c>
       <c r="Z23" s="12">
         <f t="shared" si="9"/>
-        <v>9.6441595789364953E-6</v>
+        <v>1.5313426812789355E-2</v>
       </c>
     </row>
     <row r="24" spans="2:26" x14ac:dyDescent="0.2">
@@ -2144,7 +2166,7 @@
         <v>10000</v>
       </c>
       <c r="D24" s="15" t="str">
-        <f>$C$15&amp;"-siskas"</f>
+        <f>$C$16&amp;"-siskas"</f>
         <v>USD-siskas</v>
       </c>
       <c r="F24" s="15">
@@ -2152,11 +2174,11 @@
       </c>
       <c r="G24" s="30">
         <f t="shared" si="1"/>
-        <v>120.00001</v>
+        <v>121.1</v>
       </c>
       <c r="H24" s="31">
         <f t="shared" si="5"/>
-        <v>0.49930274374586436</v>
+        <v>0.48031878424238839</v>
       </c>
       <c r="I24" s="17">
         <v>0</v>
@@ -2186,15 +2208,15 @@
       </c>
       <c r="X24" s="25">
         <f t="shared" si="4"/>
-        <v>1.7477631310876874E-3</v>
+        <v>4.9353520215909157E-2</v>
       </c>
       <c r="Y24" s="12">
         <f t="shared" si="8"/>
-        <v>1.771937494658698E-3</v>
+        <v>8.7994430047444575E-2</v>
       </c>
       <c r="Z24" s="12">
         <f t="shared" si="9"/>
-        <v>9.6441607957409303E-6</v>
+        <v>1.5378232667764835E-2</v>
       </c>
     </row>
     <row r="25" spans="2:26" x14ac:dyDescent="0.2">
@@ -2206,18 +2228,18 @@
         <v>10000</v>
       </c>
       <c r="D25" s="15" t="str">
-        <f>$C$15&amp;"-siskas"</f>
+        <f>$C$16&amp;"-siskas"</f>
         <v>USD-siskas</v>
       </c>
       <c r="E25" s="24" t="s">
-        <v>36</v>
+        <v>72</v>
       </c>
       <c r="F25" s="5">
         <v>0</v>
       </c>
       <c r="G25" s="29">
         <f>$C$13</f>
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="H25" s="32">
         <f>1/2</f>
@@ -2250,15 +2272,15 @@
       <c r="W25" s="23"/>
       <c r="X25" s="22">
         <f t="shared" si="4"/>
-        <v>1.7235887655021468E-3</v>
+        <v>1.0680688935200024E-2</v>
       </c>
       <c r="Y25" s="22">
         <f t="shared" si="8"/>
-        <v>1.7477631310876874E-3</v>
+        <v>4.9353520215909157E-2</v>
       </c>
       <c r="Z25" s="22">
         <f t="shared" si="9"/>
-        <v>9.6441620067722056E-6</v>
+        <v>1.5420318369512964E-2</v>
       </c>
     </row>
     <row r="26" spans="2:26" x14ac:dyDescent="0.2">
@@ -2266,61 +2288,40 @@
         <v>30</v>
       </c>
       <c r="C26" s="15">
-        <f>SUM(U3:U24)</f>
-        <v>1</v>
+        <f>SUM(U4:U24)</f>
+        <v>2</v>
       </c>
       <c r="D26" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="F26" s="15">
-        <f>1</f>
-        <v>1</v>
-      </c>
-      <c r="G26" s="30">
-        <f t="shared" ref="G26:G45" si="10">G25-$C$14</f>
-        <v>119.99999</v>
-      </c>
-      <c r="H26" s="31">
-        <f t="shared" ref="H26:H45" si="11">_xlfn.NORM.DIST(X26,0,1,TRUE)</f>
-        <v>0.50067796792891639</v>
-      </c>
-      <c r="I26" s="17">
-        <v>0</v>
-      </c>
-      <c r="J26" s="16">
-        <v>0</v>
-      </c>
-      <c r="K26" s="15">
-        <f t="shared" ref="K26:K45" si="12">IF(H26&lt;0.0000000001,0,CEILING($C$25*V26/H26/G26,1))</f>
-        <v>0</v>
-      </c>
-      <c r="L26" s="15">
-        <f t="shared" ref="L26:L45" si="13">K26+I26</f>
-        <v>0</v>
-      </c>
-      <c r="M26" s="14">
-        <f>L26*$G$25*RiskFactors!$C$25</f>
-        <v>0</v>
-      </c>
-      <c r="U26" s="11">
-        <f t="shared" ref="U26:U45" si="14">IF(H26&lt;0.0000000001,0,J26)</f>
-        <v>0</v>
-      </c>
-      <c r="V26" s="11">
-        <f t="shared" ref="V26:V45" si="15">IF(H26&lt;0.0000000001,0,J26/$C$27)</f>
-        <v>0</v>
-      </c>
-      <c r="X26" s="12">
-        <f t="shared" si="4"/>
-        <v>1.6994143979020754E-3</v>
-      </c>
-      <c r="Y26" s="12">
-        <f t="shared" si="8"/>
-        <v>1.7235887655021468E-3</v>
-      </c>
-      <c r="Z26" s="12">
-        <f t="shared" si="9"/>
-        <v>9.6441632124744103E-6</v>
+      <c r="E26" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="F26" s="5">
+        <v>0</v>
+      </c>
+      <c r="G26" s="29">
+        <f>C14</f>
+        <v>119</v>
+      </c>
+      <c r="H26" s="32">
+        <f>1/2</f>
+        <v>0.5</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="J26" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K26" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="L26" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="M26" s="5" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="2:26" x14ac:dyDescent="0.2">
@@ -2328,23 +2329,23 @@
         <v>29</v>
       </c>
       <c r="C27" s="15">
-        <f>SUM(U26:U45)</f>
+        <f>SUM(U27:U46)</f>
         <v>1</v>
       </c>
       <c r="D27" s="21" t="s">
         <v>28</v>
       </c>
       <c r="F27" s="15">
-        <f t="shared" ref="F27:F45" si="16">1+F26</f>
-        <v>2</v>
+        <f>1</f>
+        <v>1</v>
       </c>
       <c r="G27" s="30">
-        <f t="shared" si="10"/>
-        <v>119.99997999999999</v>
+        <f t="shared" ref="G27:G46" si="10">G26-$C$15</f>
+        <v>118.9</v>
       </c>
       <c r="H27" s="31">
-        <f t="shared" si="11"/>
-        <v>0.50066832376450421</v>
+        <f>_xlfn.NORM.DIST(X27,0,1,TRUE)</f>
+        <v>0.4885619410960117</v>
       </c>
       <c r="I27" s="17">
         <v>0</v>
@@ -2353,11 +2354,11 @@
         <v>0</v>
       </c>
       <c r="K27" s="15">
-        <f t="shared" si="12"/>
+        <f t="shared" ref="K27:K46" si="11">IF(H27&lt;0.0000000001,0,CEILING($C$25*V27/H27/G27,1))</f>
         <v>0</v>
       </c>
       <c r="L27" s="15">
-        <f t="shared" si="13"/>
+        <f t="shared" ref="L27:L46" si="12">K27+I27</f>
         <v>0</v>
       </c>
       <c r="M27" s="14">
@@ -2365,24 +2366,24 @@
         <v>0</v>
       </c>
       <c r="U27" s="11">
-        <f t="shared" si="14"/>
+        <f t="shared" ref="U27:U46" si="13">IF(H27&lt;0.0000000001,0,J27)</f>
         <v>0</v>
       </c>
       <c r="V27" s="11">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="V27:V46" si="14">IF(H27&lt;0.0000000001,0,J27/$C$27)</f>
         <v>0</v>
       </c>
       <c r="X27" s="12">
-        <f t="shared" si="4"/>
-        <v>1.6752400282874732E-3</v>
+        <f>(LN(G27/$C$14)-($C$7-0.5*$C$8*$C$8)*$C$10)/($C$8*SQRT($C$10))</f>
+        <v>-2.8674891022877427E-2</v>
       </c>
       <c r="Y27" s="12">
-        <f t="shared" si="8"/>
-        <v>1.6994143979020754E-3</v>
+        <f>(LN(G26/$C$14)-($C$7-0.5*$C$8*$C$8)*$C$10)/($C$8*SQRT($C$10))</f>
+        <v>1.0680688935200024E-2</v>
       </c>
       <c r="Z27" s="12">
-        <f t="shared" si="9"/>
-        <v>9.6441644121814107E-6</v>
+        <f>_xlfn.NORM.DIST(Y27,0,1,TRUE)-_xlfn.NORM.DIST(X27,0,1,TRUE)</f>
+        <v>1.5698956292086952E-2</v>
       </c>
     </row>
     <row r="28" spans="2:26" x14ac:dyDescent="0.2">
@@ -2390,36 +2391,36 @@
         <v>27</v>
       </c>
       <c r="C28" s="20">
-        <f>SUMPRODUCT(G3:G33,H3:H33,L3:L33)</f>
-        <v>10004.295901619131</v>
+        <f>SUMPRODUCT(G3:G34,H3:H34,L3:L34)</f>
+        <v>10034.049122395518</v>
       </c>
       <c r="D28" s="19" t="s">
         <v>25</v>
       </c>
       <c r="F28" s="15">
-        <f t="shared" si="16"/>
-        <v>3</v>
+        <f t="shared" ref="F28:F46" si="15">1+F27</f>
+        <v>2</v>
       </c>
       <c r="G28" s="30">
         <f t="shared" si="10"/>
-        <v>119.99996999999999</v>
+        <v>118.80000000000001</v>
       </c>
       <c r="H28" s="31">
+        <f t="shared" ref="H27:H46" si="16">_xlfn.NORM.DIST(X28,0,1,TRUE)</f>
+        <v>0.47286750917599063</v>
+      </c>
+      <c r="I28" s="17">
+        <v>0</v>
+      </c>
+      <c r="J28" s="16">
+        <v>0</v>
+      </c>
+      <c r="K28" s="15">
         <f t="shared" si="11"/>
-        <v>0.50065867959889765</v>
-      </c>
-      <c r="I28" s="17">
-        <v>0</v>
-      </c>
-      <c r="J28" s="16">
-        <v>0</v>
-      </c>
-      <c r="K28" s="15">
+        <v>0</v>
+      </c>
+      <c r="L28" s="15">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="L28" s="15">
-        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="M28" s="14">
@@ -2427,24 +2428,24 @@
         <v>0</v>
       </c>
       <c r="U28" s="11">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="V28" s="11">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="V28" s="11">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
       <c r="X28" s="12">
-        <f t="shared" si="4"/>
-        <v>1.6510656566583399E-3</v>
+        <f t="shared" ref="X28:X46" si="17">(LN(G28/$C$14)-($C$7-0.5*$C$8*$C$8)*$C$10)/($C$8*SQRT($C$10))</f>
+        <v>-6.8063584640688624E-2</v>
       </c>
       <c r="Y28" s="12">
-        <f t="shared" si="8"/>
-        <v>1.6752400282874732E-3</v>
+        <f t="shared" ref="Y28:Y46" si="18">(LN(G27/$C$14)-($C$7-0.5*$C$8*$C$8)*$C$10)/($C$8*SQRT($C$10))</f>
+        <v>-2.8674891022877427E-2</v>
       </c>
       <c r="Z28" s="12">
-        <f t="shared" si="9"/>
-        <v>9.6441656065593406E-6</v>
+        <f t="shared" ref="Z27:Z46" si="19">_xlfn.NORM.DIST(Y28,0,1,TRUE)-_xlfn.NORM.DIST(X28,0,1,TRUE)</f>
+        <v>1.5694431920021068E-2</v>
       </c>
     </row>
     <row r="29" spans="2:26" x14ac:dyDescent="0.2">
@@ -2452,36 +2453,36 @@
         <v>26</v>
       </c>
       <c r="C29" s="20">
-        <f>SUMPRODUCT(G26:G177,H26:H177,L26:L177)</f>
-        <v>10031.838695077195</v>
+        <f>SUMPRODUCT(G27:G177,H27:H177,L27:L177)</f>
+        <v>10004.634424545298</v>
       </c>
       <c r="D29" s="19" t="s">
         <v>25</v>
       </c>
       <c r="F29" s="15">
-        <f t="shared" si="16"/>
-        <v>4</v>
+        <f t="shared" si="15"/>
+        <v>3</v>
       </c>
       <c r="G29" s="30">
         <f t="shared" si="10"/>
-        <v>119.99995999999999</v>
+        <v>118.70000000000002</v>
       </c>
       <c r="H29" s="31">
+        <f t="shared" si="16"/>
+        <v>0.45720193475010851</v>
+      </c>
+      <c r="I29" s="17">
+        <v>0</v>
+      </c>
+      <c r="J29" s="16">
+        <v>0</v>
+      </c>
+      <c r="K29" s="15">
         <f t="shared" si="11"/>
-        <v>0.50064903543208972</v>
-      </c>
-      <c r="I29" s="17">
-        <v>0</v>
-      </c>
-      <c r="J29" s="16">
-        <v>0</v>
-      </c>
-      <c r="K29" s="15">
+        <v>0</v>
+      </c>
+      <c r="L29" s="15">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="L29" s="15">
-        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="M29" s="14">
@@ -2489,51 +2490,51 @@
         <v>0</v>
       </c>
       <c r="U29" s="11">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="V29" s="11">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="V29" s="11">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
       <c r="X29" s="12">
-        <f t="shared" si="4"/>
-        <v>1.6268912829824683E-3</v>
+        <f t="shared" si="17"/>
+        <v>-0.10748544768862817</v>
       </c>
       <c r="Y29" s="12">
-        <f t="shared" si="8"/>
-        <v>1.6510656566583399E-3</v>
+        <f t="shared" si="18"/>
+        <v>-6.8063584640688624E-2</v>
       </c>
       <c r="Z29" s="12">
-        <f t="shared" si="9"/>
-        <v>9.6441668079316756E-6</v>
+        <f t="shared" si="19"/>
+        <v>1.5665574425882123E-2</v>
       </c>
     </row>
     <row r="30" spans="2:26" x14ac:dyDescent="0.2">
       <c r="F30" s="15">
-        <f t="shared" si="16"/>
-        <v>5</v>
+        <f t="shared" si="15"/>
+        <v>4</v>
       </c>
       <c r="G30" s="30">
         <f t="shared" si="10"/>
-        <v>119.99994999999998</v>
+        <v>118.60000000000002</v>
       </c>
       <c r="H30" s="31">
+        <f t="shared" si="16"/>
+        <v>0.44158947800345705</v>
+      </c>
+      <c r="I30" s="17">
+        <v>0</v>
+      </c>
+      <c r="J30" s="16">
+        <v>0</v>
+      </c>
+      <c r="K30" s="15">
         <f t="shared" si="11"/>
-        <v>0.50063939126411161</v>
-      </c>
-      <c r="I30" s="17">
-        <v>0</v>
-      </c>
-      <c r="J30" s="16">
-        <v>0</v>
-      </c>
-      <c r="K30" s="15">
+        <v>0</v>
+      </c>
+      <c r="L30" s="15">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="L30" s="15">
-        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="M30" s="14">
@@ -2541,24 +2542,24 @@
         <v>0</v>
       </c>
       <c r="U30" s="11">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="V30" s="11">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="V30" s="11">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
       <c r="X30" s="12">
-        <f t="shared" si="4"/>
-        <v>1.6027169073242714E-3</v>
+        <f t="shared" si="17"/>
+        <v>-0.14694053607808216</v>
       </c>
       <c r="Y30" s="12">
-        <f t="shared" si="8"/>
-        <v>1.6268912829824683E-3</v>
+        <f t="shared" si="18"/>
+        <v>-0.10748544768862817</v>
       </c>
       <c r="Z30" s="12">
-        <f t="shared" si="9"/>
-        <v>9.6441679781067435E-6</v>
+        <f t="shared" si="19"/>
+        <v>1.561245674665146E-2</v>
       </c>
     </row>
     <row r="31" spans="2:26" x14ac:dyDescent="0.2">
@@ -2568,29 +2569,29 @@
       <c r="C31" s="4"/>
       <c r="D31" s="5"/>
       <c r="F31" s="15">
-        <f t="shared" si="16"/>
-        <v>6</v>
+        <f t="shared" si="15"/>
+        <v>5</v>
       </c>
       <c r="G31" s="30">
         <f t="shared" si="10"/>
-        <v>119.99993999999998</v>
+        <v>118.50000000000003</v>
       </c>
       <c r="H31" s="31">
+        <f t="shared" si="16"/>
+        <v>0.4260542130801106</v>
+      </c>
+      <c r="I31" s="17">
+        <v>0</v>
+      </c>
+      <c r="J31" s="16">
+        <v>0</v>
+      </c>
+      <c r="K31" s="15">
         <f t="shared" si="11"/>
-        <v>0.50062974709495622</v>
-      </c>
-      <c r="I31" s="17">
-        <v>0</v>
-      </c>
-      <c r="J31" s="16">
-        <v>0</v>
-      </c>
-      <c r="K31" s="15">
+        <v>0</v>
+      </c>
+      <c r="L31" s="15">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="L31" s="15">
-        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="M31" s="14">
@@ -2598,24 +2599,24 @@
         <v>0</v>
       </c>
       <c r="U31" s="11">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="V31" s="11">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="V31" s="11">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
       <c r="X31" s="12">
-        <f t="shared" si="4"/>
-        <v>1.5785425296515423E-3</v>
+        <f t="shared" si="17"/>
+        <v>-0.1864289058619458</v>
       </c>
       <c r="Y31" s="12">
-        <f t="shared" si="8"/>
-        <v>1.6027169073242714E-3</v>
+        <f t="shared" si="18"/>
+        <v>-0.14694053607808216</v>
       </c>
       <c r="Z31" s="12">
-        <f t="shared" si="9"/>
-        <v>9.6441691553872388E-6</v>
+        <f t="shared" si="19"/>
+        <v>1.5535264923346448E-2</v>
       </c>
     </row>
     <row r="32" spans="2:26" x14ac:dyDescent="0.2">
@@ -2623,37 +2624,37 @@
         <v>23</v>
       </c>
       <c r="C32" s="18">
-        <f>SUM(M3:M33)</f>
-        <v>233.84628325664463</v>
+        <f>SUM(M3:M34)</f>
+        <v>1925.1415065758192</v>
       </c>
       <c r="D32" s="15" t="str">
-        <f>C15</f>
+        <f>C16</f>
         <v>USD</v>
       </c>
       <c r="F32" s="15">
-        <f t="shared" si="16"/>
-        <v>7</v>
+        <f t="shared" si="15"/>
+        <v>6</v>
       </c>
       <c r="G32" s="30">
         <f t="shared" si="10"/>
-        <v>119.99992999999998</v>
+        <v>118.40000000000003</v>
       </c>
       <c r="H32" s="31">
+        <f t="shared" si="16"/>
+        <v>0.41061991594866376</v>
+      </c>
+      <c r="I32" s="17">
+        <v>0</v>
+      </c>
+      <c r="J32" s="16">
+        <v>0</v>
+      </c>
+      <c r="K32" s="15">
         <f t="shared" si="11"/>
-        <v>0.50062010292462911</v>
-      </c>
-      <c r="I32" s="17">
-        <v>0</v>
-      </c>
-      <c r="J32" s="16">
-        <v>0</v>
-      </c>
-      <c r="K32" s="15">
+        <v>0</v>
+      </c>
+      <c r="L32" s="15">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="L32" s="15">
-        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="M32" s="14">
@@ -2661,24 +2662,24 @@
         <v>0</v>
       </c>
       <c r="U32" s="11">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="V32" s="11">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="V32" s="11">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
       <c r="X32" s="12">
-        <f t="shared" si="4"/>
-        <v>1.5543681499642806E-3</v>
+        <f t="shared" si="17"/>
+        <v>-0.22595061323506455</v>
       </c>
       <c r="Y32" s="12">
-        <f t="shared" si="8"/>
-        <v>1.5785425296515423E-3</v>
+        <f t="shared" si="18"/>
+        <v>-0.1864289058619458</v>
       </c>
       <c r="Z32" s="12">
-        <f t="shared" si="9"/>
-        <v>9.644170327116619E-6</v>
+        <f t="shared" si="19"/>
+        <v>1.5434297131446839E-2</v>
       </c>
     </row>
     <row r="33" spans="2:26" x14ac:dyDescent="0.2">
@@ -2686,37 +2687,37 @@
         <v>22</v>
       </c>
       <c r="C33" s="18">
-        <f>SUM(M26:M177)</f>
-        <v>699.36888308002551</v>
+        <f>SUM(M27:M177)</f>
+        <v>4964.0801528466282</v>
       </c>
       <c r="D33" s="15" t="str">
-        <f>C15</f>
+        <f>C16</f>
         <v>USD</v>
       </c>
       <c r="F33" s="15">
-        <f t="shared" si="16"/>
-        <v>8</v>
+        <f t="shared" si="15"/>
+        <v>7</v>
       </c>
       <c r="G33" s="30">
         <f t="shared" si="10"/>
-        <v>119.99991999999997</v>
+        <v>118.30000000000004</v>
       </c>
       <c r="H33" s="31">
+        <f t="shared" si="16"/>
+        <v>0.39530995411141673</v>
+      </c>
+      <c r="I33" s="17">
+        <v>0</v>
+      </c>
+      <c r="J33" s="16">
+        <v>0</v>
+      </c>
+      <c r="K33" s="15">
         <f t="shared" si="11"/>
-        <v>0.50061045875313592</v>
-      </c>
-      <c r="I33" s="17">
-        <v>0</v>
-      </c>
-      <c r="J33" s="16">
-        <v>0</v>
-      </c>
-      <c r="K33" s="15">
+        <v>0</v>
+      </c>
+      <c r="L33" s="15">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="L33" s="15">
-        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="M33" s="14">
@@ -2724,51 +2725,51 @@
         <v>0</v>
       </c>
       <c r="U33" s="11">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="V33" s="11">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="V33" s="11">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
       <c r="X33" s="12">
-        <f t="shared" si="4"/>
-        <v>1.5301937682624862E-3</v>
+        <f t="shared" si="17"/>
+        <v>-0.26550571453472971</v>
       </c>
       <c r="Y33" s="12">
-        <f t="shared" si="8"/>
-        <v>1.5543681499642806E-3</v>
+        <f t="shared" si="18"/>
+        <v>-0.22595061323506455</v>
       </c>
       <c r="Z33" s="12">
-        <f t="shared" si="9"/>
-        <v>9.6441714931838618E-6</v>
+        <f t="shared" si="19"/>
+        <v>1.5309961837247033E-2</v>
       </c>
     </row>
     <row r="34" spans="2:26" x14ac:dyDescent="0.2">
       <c r="F34" s="15">
-        <f t="shared" si="16"/>
-        <v>9</v>
+        <f t="shared" si="15"/>
+        <v>8</v>
       </c>
       <c r="G34" s="30">
         <f t="shared" si="10"/>
-        <v>119.99990999999997</v>
+        <v>118.20000000000005</v>
       </c>
       <c r="H34" s="31">
+        <f t="shared" si="16"/>
+        <v>0.38014717901643136</v>
+      </c>
+      <c r="I34" s="17">
+        <v>0</v>
+      </c>
+      <c r="J34" s="16">
+        <v>0</v>
+      </c>
+      <c r="K34" s="15">
         <f t="shared" si="11"/>
-        <v>0.50060081458048222</v>
-      </c>
-      <c r="I34" s="17">
-        <v>0</v>
-      </c>
-      <c r="J34" s="16">
-        <v>0</v>
-      </c>
-      <c r="K34" s="15">
+        <v>0</v>
+      </c>
+      <c r="L34" s="15">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="L34" s="15">
-        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="M34" s="14">
@@ -2776,24 +2777,24 @@
         <v>0</v>
       </c>
       <c r="U34" s="11">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="V34" s="11">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="V34" s="11">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
       <c r="X34" s="12">
-        <f t="shared" si="4"/>
-        <v>1.5060193845461585E-3</v>
+        <f t="shared" si="17"/>
+        <v>-0.3050942662411758</v>
       </c>
       <c r="Y34" s="12">
-        <f t="shared" si="8"/>
-        <v>1.5301937682624862E-3</v>
+        <f t="shared" si="18"/>
+        <v>-0.26550571453472971</v>
       </c>
       <c r="Z34" s="12">
-        <f t="shared" si="9"/>
-        <v>9.6441726536999894E-6</v>
+        <f t="shared" si="19"/>
+        <v>1.516277509498537E-2</v>
       </c>
     </row>
     <row r="35" spans="2:26" x14ac:dyDescent="0.2">
@@ -2803,54 +2804,54 @@
       <c r="C35" s="4"/>
       <c r="D35" s="5"/>
       <c r="F35" s="15">
-        <f t="shared" si="16"/>
-        <v>10</v>
+        <f t="shared" si="15"/>
+        <v>9</v>
       </c>
       <c r="G35" s="30">
         <f t="shared" si="10"/>
-        <v>119.99989999999997</v>
+        <v>118.10000000000005</v>
       </c>
       <c r="H35" s="31">
+        <f t="shared" si="16"/>
+        <v>0.36515382200733265</v>
+      </c>
+      <c r="I35" s="17">
+        <v>0</v>
+      </c>
+      <c r="J35" s="16">
+        <v>0</v>
+      </c>
+      <c r="K35" s="15">
         <f t="shared" si="11"/>
-        <v>0.50059117040667378</v>
-      </c>
-      <c r="I35" s="17">
-        <v>0</v>
-      </c>
-      <c r="J35" s="16">
-        <v>1</v>
-      </c>
-      <c r="K35" s="15">
+        <v>0</v>
+      </c>
+      <c r="L35" s="15">
         <f t="shared" si="12"/>
-        <v>167</v>
-      </c>
-      <c r="L35" s="15">
-        <f t="shared" si="13"/>
-        <v>167</v>
+        <v>0</v>
       </c>
       <c r="M35" s="14">
         <f>L35*$G$25*RiskFactors!$C$25</f>
-        <v>231.36844145447154</v>
+        <v>0</v>
       </c>
       <c r="U35" s="11">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="V35" s="11">
         <f t="shared" si="14"/>
-        <v>1</v>
-      </c>
-      <c r="V35" s="11">
-        <f t="shared" si="15"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X35" s="12">
-        <f t="shared" si="4"/>
-        <v>1.4818449988152969E-3</v>
+        <f t="shared" si="17"/>
+        <v>-0.34471632497802812</v>
       </c>
       <c r="Y35" s="12">
-        <f t="shared" si="8"/>
-        <v>1.5060193845461585E-3</v>
+        <f t="shared" si="18"/>
+        <v>-0.3050942662411758</v>
       </c>
       <c r="Z35" s="12">
-        <f t="shared" si="9"/>
-        <v>9.6441738084429574E-6</v>
+        <f t="shared" si="19"/>
+        <v>1.4993357009098707E-2</v>
       </c>
     </row>
     <row r="36" spans="2:26" x14ac:dyDescent="0.2">
@@ -2859,88 +2860,88 @@
       </c>
       <c r="C36" s="14">
         <f>C20+SUM(C32:C33)</f>
-        <v>10933.215166336669</v>
+        <v>16889.221659422448</v>
       </c>
       <c r="D36" s="15" t="str">
-        <f>C15</f>
+        <f>C16</f>
         <v>USD</v>
       </c>
       <c r="F36" s="15">
-        <f t="shared" si="16"/>
-        <v>11</v>
+        <f t="shared" si="15"/>
+        <v>10</v>
       </c>
       <c r="G36" s="30">
         <f t="shared" si="10"/>
-        <v>119.99988999999997</v>
+        <v>118.00000000000006</v>
       </c>
       <c r="H36" s="31">
+        <f t="shared" si="16"/>
+        <v>0.3503513946121759</v>
+      </c>
+      <c r="I36" s="17">
+        <v>0</v>
+      </c>
+      <c r="J36" s="16">
+        <v>1</v>
+      </c>
+      <c r="K36" s="15">
         <f t="shared" si="11"/>
-        <v>0.50058152623171615</v>
-      </c>
-      <c r="I36" s="17">
-        <v>0</v>
-      </c>
-      <c r="J36" s="16">
-        <v>0</v>
-      </c>
-      <c r="K36" s="15">
+        <v>242</v>
+      </c>
+      <c r="L36" s="15">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="L36" s="15">
-        <f t="shared" si="13"/>
-        <v>0</v>
+        <v>242</v>
       </c>
       <c r="M36" s="14">
         <f>L36*$G$25*RiskFactors!$C$25</f>
-        <v>0</v>
+        <v>2037.967060226518</v>
       </c>
       <c r="U36" s="11">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="V36" s="11">
         <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="V36" s="11">
-        <f t="shared" si="15"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X36" s="12">
-        <f t="shared" si="4"/>
-        <v>1.4576706110699018E-3</v>
+        <f t="shared" si="17"/>
+        <v>-0.38437194751283016</v>
       </c>
       <c r="Y36" s="12">
-        <f t="shared" si="8"/>
-        <v>1.4818449988152969E-3</v>
+        <f t="shared" si="18"/>
+        <v>-0.34471632497802812</v>
       </c>
       <c r="Z36" s="12">
-        <f t="shared" si="9"/>
-        <v>9.6441749576348101E-6</v>
+        <f t="shared" si="19"/>
+        <v>1.4802427395156748E-2</v>
       </c>
     </row>
     <row r="37" spans="2:26" x14ac:dyDescent="0.2">
       <c r="F37" s="15">
-        <f t="shared" si="16"/>
-        <v>12</v>
+        <f t="shared" si="15"/>
+        <v>11</v>
       </c>
       <c r="G37" s="30">
         <f t="shared" si="10"/>
-        <v>119.99987999999996</v>
+        <v>117.90000000000006</v>
       </c>
       <c r="H37" s="31">
+        <f t="shared" si="16"/>
+        <v>0.33576059393057073</v>
+      </c>
+      <c r="I37" s="17">
+        <v>0</v>
+      </c>
+      <c r="J37" s="16">
+        <v>0</v>
+      </c>
+      <c r="K37" s="15">
         <f t="shared" si="11"/>
-        <v>0.50057188205560221</v>
-      </c>
-      <c r="I37" s="17">
-        <v>0</v>
-      </c>
-      <c r="J37" s="16">
-        <v>0</v>
-      </c>
-      <c r="K37" s="15">
+        <v>0</v>
+      </c>
+      <c r="L37" s="15">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="L37" s="15">
-        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="M37" s="14">
@@ -2948,51 +2949,51 @@
         <v>0</v>
       </c>
       <c r="U37" s="11">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="V37" s="11">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="V37" s="11">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
       <c r="X37" s="12">
-        <f t="shared" si="4"/>
-        <v>1.4334962212777657E-3</v>
+        <f t="shared" si="17"/>
+        <v>-0.42406119075749521</v>
       </c>
       <c r="Y37" s="12">
-        <f t="shared" si="8"/>
-        <v>1.4576706110699018E-3</v>
+        <f t="shared" si="18"/>
+        <v>-0.38437194751283016</v>
       </c>
       <c r="Z37" s="12">
-        <f t="shared" si="9"/>
-        <v>9.6441761139320903E-6</v>
+        <f t="shared" si="19"/>
+        <v>1.4590800681605176E-2</v>
       </c>
     </row>
     <row r="38" spans="2:26" x14ac:dyDescent="0.2">
       <c r="F38" s="15">
-        <f t="shared" si="16"/>
-        <v>13</v>
+        <f t="shared" si="15"/>
+        <v>12</v>
       </c>
       <c r="G38" s="30">
         <f t="shared" si="10"/>
-        <v>119.99986999999996</v>
+        <v>117.80000000000007</v>
       </c>
       <c r="H38" s="31">
+        <f t="shared" si="16"/>
+        <v>0.32140121382768483</v>
+      </c>
+      <c r="I38" s="17">
+        <v>0</v>
+      </c>
+      <c r="J38" s="16">
+        <v>0</v>
+      </c>
+      <c r="K38" s="15">
         <f t="shared" si="11"/>
-        <v>0.50056223787836318</v>
-      </c>
-      <c r="I38" s="17">
-        <v>0</v>
-      </c>
-      <c r="J38" s="16">
-        <v>0</v>
-      </c>
-      <c r="K38" s="15">
+        <v>0</v>
+      </c>
+      <c r="L38" s="15">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="L38" s="15">
-        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="M38" s="14">
@@ -3000,51 +3001,51 @@
         <v>0</v>
       </c>
       <c r="U38" s="11">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="V38" s="11">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="V38" s="11">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
       <c r="X38" s="12">
-        <f t="shared" si="4"/>
-        <v>1.4093218295033014E-3</v>
+        <f t="shared" si="17"/>
+        <v>-0.46378411176881223</v>
       </c>
       <c r="Y38" s="12">
-        <f t="shared" si="8"/>
-        <v>1.4334962212777657E-3</v>
+        <f t="shared" si="18"/>
+        <v>-0.42406119075749521</v>
       </c>
       <c r="Z38" s="12">
-        <f t="shared" si="9"/>
-        <v>9.6441772390321034E-6</v>
+        <f t="shared" si="19"/>
+        <v>1.4359380102885899E-2</v>
       </c>
     </row>
     <row r="39" spans="2:26" x14ac:dyDescent="0.2">
       <c r="F39" s="15">
-        <f t="shared" si="16"/>
-        <v>14</v>
+        <f t="shared" si="15"/>
+        <v>13</v>
       </c>
       <c r="G39" s="30">
         <f t="shared" si="10"/>
-        <v>119.99985999999996</v>
+        <v>117.70000000000007</v>
       </c>
       <c r="H39" s="31">
+        <f t="shared" si="16"/>
+        <v>0.30729206258577813</v>
+      </c>
+      <c r="I39" s="17">
+        <v>0</v>
+      </c>
+      <c r="J39" s="16">
+        <v>0</v>
+      </c>
+      <c r="K39" s="15">
         <f t="shared" si="11"/>
-        <v>0.50055259369999194</v>
-      </c>
-      <c r="I39" s="17">
-        <v>0</v>
-      </c>
-      <c r="J39" s="16">
-        <v>0</v>
-      </c>
-      <c r="K39" s="15">
+        <v>0</v>
+      </c>
+      <c r="L39" s="15">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="L39" s="15">
-        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="M39" s="14">
@@ -3052,51 +3053,51 @@
         <v>0</v>
       </c>
       <c r="U39" s="11">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="V39" s="11">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="V39" s="11">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
       <c r="X39" s="12">
-        <f t="shared" si="4"/>
-        <v>1.3851474357143023E-3</v>
+        <f t="shared" si="17"/>
+        <v>-0.5035407677489534</v>
       </c>
       <c r="Y39" s="12">
-        <f t="shared" si="8"/>
-        <v>1.4093218295033014E-3</v>
+        <f t="shared" si="18"/>
+        <v>-0.46378411176881223</v>
       </c>
       <c r="Z39" s="12">
-        <f t="shared" si="9"/>
-        <v>9.644178371237544E-6</v>
+        <f t="shared" si="19"/>
+        <v>1.4109151241906703E-2</v>
       </c>
     </row>
     <row r="40" spans="2:26" x14ac:dyDescent="0.2">
       <c r="F40" s="15">
-        <f t="shared" si="16"/>
-        <v>15</v>
+        <f t="shared" si="15"/>
+        <v>14</v>
       </c>
       <c r="G40" s="30">
         <f t="shared" si="10"/>
-        <v>119.99984999999995</v>
+        <v>117.60000000000008</v>
       </c>
       <c r="H40" s="31">
+        <f t="shared" si="16"/>
+        <v>0.29345088759903015</v>
+      </c>
+      <c r="I40" s="17">
+        <v>0</v>
+      </c>
+      <c r="J40" s="16">
+        <v>0</v>
+      </c>
+      <c r="K40" s="15">
         <f t="shared" si="11"/>
-        <v>0.50054294952049405</v>
-      </c>
-      <c r="I40" s="17">
-        <v>0</v>
-      </c>
-      <c r="J40" s="16">
-        <v>0</v>
-      </c>
-      <c r="K40" s="15">
+        <v>0</v>
+      </c>
+      <c r="L40" s="15">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="L40" s="15">
-        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="M40" s="14">
@@ -3104,51 +3105,51 @@
         <v>0</v>
       </c>
       <c r="U40" s="11">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="V40" s="11">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="V40" s="11">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
       <c r="X40" s="12">
-        <f t="shared" si="4"/>
-        <v>1.3609730399107682E-3</v>
+        <f t="shared" si="17"/>
+        <v>-0.54333121604593182</v>
       </c>
       <c r="Y40" s="12">
-        <f t="shared" si="8"/>
-        <v>1.3851474357143023E-3</v>
+        <f t="shared" si="18"/>
+        <v>-0.5035407677489534</v>
       </c>
       <c r="Z40" s="12">
-        <f t="shared" si="9"/>
-        <v>9.6441794978918693E-6</v>
+        <f t="shared" si="19"/>
+        <v>1.3841174986747973E-2</v>
       </c>
     </row>
     <row r="41" spans="2:26" x14ac:dyDescent="0.2">
       <c r="F41" s="15">
-        <f t="shared" si="16"/>
-        <v>16</v>
+        <f t="shared" si="15"/>
+        <v>15</v>
       </c>
       <c r="G41" s="30">
         <f t="shared" si="10"/>
-        <v>119.99983999999995</v>
+        <v>117.50000000000009</v>
       </c>
       <c r="H41" s="31">
+        <f t="shared" si="16"/>
+        <v>0.27989430762648004</v>
+      </c>
+      <c r="I41" s="17">
+        <v>0</v>
+      </c>
+      <c r="J41" s="16">
+        <v>0</v>
+      </c>
+      <c r="K41" s="15">
         <f t="shared" si="11"/>
-        <v>0.50053330533987517</v>
-      </c>
-      <c r="I41" s="17">
-        <v>0</v>
-      </c>
-      <c r="J41" s="16">
-        <v>0</v>
-      </c>
-      <c r="K41" s="15">
+        <v>0</v>
+      </c>
+      <c r="L41" s="15">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="L41" s="15">
-        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="M41" s="14">
@@ -3156,51 +3157,51 @@
         <v>0</v>
       </c>
       <c r="U41" s="11">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="V41" s="11">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="V41" s="11">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
       <c r="X41" s="12">
-        <f t="shared" si="4"/>
-        <v>1.3367986420926984E-3</v>
+        <f t="shared" si="17"/>
+        <v>-0.5831555141541398</v>
       </c>
       <c r="Y41" s="12">
-        <f t="shared" si="8"/>
-        <v>1.3609730399107682E-3</v>
+        <f t="shared" si="18"/>
+        <v>-0.54333121604593182</v>
       </c>
       <c r="Z41" s="12">
-        <f t="shared" si="9"/>
-        <v>9.6441806188840573E-6</v>
+        <f t="shared" si="19"/>
+        <v>1.3556579972550109E-2</v>
       </c>
     </row>
     <row r="42" spans="2:26" x14ac:dyDescent="0.2">
       <c r="F42" s="15">
-        <f t="shared" si="16"/>
-        <v>17</v>
+        <f t="shared" si="15"/>
+        <v>16</v>
       </c>
       <c r="G42" s="30">
         <f t="shared" si="10"/>
-        <v>119.99982999999995</v>
+        <v>117.40000000000009</v>
       </c>
       <c r="H42" s="31">
+        <f t="shared" si="16"/>
+        <v>0.26663775304204262</v>
+      </c>
+      <c r="I42" s="17">
+        <v>0</v>
+      </c>
+      <c r="J42" s="16">
+        <v>0</v>
+      </c>
+      <c r="K42" s="15">
         <f t="shared" si="11"/>
-        <v>0.50052366115814095</v>
-      </c>
-      <c r="I42" s="17">
-        <v>0</v>
-      </c>
-      <c r="J42" s="16">
-        <v>0</v>
-      </c>
-      <c r="K42" s="15">
+        <v>0</v>
+      </c>
+      <c r="L42" s="15">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="L42" s="15">
-        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="M42" s="14">
@@ -3208,51 +3209,51 @@
         <v>0</v>
       </c>
       <c r="U42" s="11">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="V42" s="11">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="V42" s="11">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
       <c r="X42" s="12">
-        <f t="shared" si="4"/>
-        <v>1.3126242422600925E-3</v>
+        <f t="shared" si="17"/>
+        <v>-0.6230137197148109</v>
       </c>
       <c r="Y42" s="12">
-        <f t="shared" si="8"/>
-        <v>1.3367986420926984E-3</v>
+        <f t="shared" si="18"/>
+        <v>-0.5831555141541398</v>
       </c>
       <c r="Z42" s="12">
-        <f t="shared" si="9"/>
-        <v>9.6441817342141078E-6</v>
+        <f t="shared" si="19"/>
+        <v>1.3256554584437419E-2</v>
       </c>
     </row>
     <row r="43" spans="2:26" x14ac:dyDescent="0.2">
       <c r="F43" s="15">
-        <f t="shared" si="16"/>
-        <v>18</v>
+        <f t="shared" si="15"/>
+        <v>17</v>
       </c>
       <c r="G43" s="30">
         <f t="shared" si="10"/>
-        <v>119.99981999999994</v>
+        <v>117.3000000000001</v>
       </c>
       <c r="H43" s="31">
+        <f t="shared" si="16"/>
+        <v>0.25369541444041321</v>
+      </c>
+      <c r="I43" s="17">
+        <v>0</v>
+      </c>
+      <c r="J43" s="16">
+        <v>0</v>
+      </c>
+      <c r="K43" s="15">
         <f t="shared" si="11"/>
-        <v>0.50051401697529707</v>
-      </c>
-      <c r="I43" s="17">
-        <v>0</v>
-      </c>
-      <c r="J43" s="16">
-        <v>0</v>
-      </c>
-      <c r="K43" s="15">
+        <v>0</v>
+      </c>
+      <c r="L43" s="15">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="L43" s="15">
-        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="M43" s="14">
@@ -3260,51 +3261,51 @@
         <v>0</v>
       </c>
       <c r="U43" s="11">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="V43" s="11">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="V43" s="11">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
       <c r="X43" s="12">
-        <f t="shared" si="4"/>
-        <v>1.2884498404129507E-3</v>
+        <f t="shared" si="17"/>
+        <v>-0.66290589051653548</v>
       </c>
       <c r="Y43" s="12">
-        <f t="shared" si="8"/>
-        <v>1.3126242422600925E-3</v>
+        <f t="shared" si="18"/>
+        <v>-0.6230137197148109</v>
       </c>
       <c r="Z43" s="12">
-        <f t="shared" si="9"/>
-        <v>9.644182843882021E-6</v>
+        <f t="shared" si="19"/>
+        <v>1.2942338601629411E-2</v>
       </c>
     </row>
     <row r="44" spans="2:26" x14ac:dyDescent="0.2">
       <c r="F44" s="15">
-        <f t="shared" si="16"/>
-        <v>19</v>
+        <f t="shared" si="15"/>
+        <v>18</v>
       </c>
       <c r="G44" s="30">
         <f t="shared" si="10"/>
-        <v>119.99980999999994</v>
+        <v>117.2000000000001</v>
       </c>
       <c r="H44" s="31">
+        <f t="shared" si="16"/>
+        <v>0.24108019987464452</v>
+      </c>
+      <c r="I44" s="17">
+        <v>0</v>
+      </c>
+      <c r="J44" s="16">
+        <v>0</v>
+      </c>
+      <c r="K44" s="15">
         <f t="shared" si="11"/>
-        <v>0.50050437279133608</v>
-      </c>
-      <c r="I44" s="17">
-        <v>0</v>
-      </c>
-      <c r="J44" s="16">
-        <v>0</v>
-      </c>
-      <c r="K44" s="15">
+        <v>0</v>
+      </c>
+      <c r="L44" s="15">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="L44" s="15">
-        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="M44" s="14">
@@ -3312,51 +3313,51 @@
         <v>0</v>
       </c>
       <c r="U44" s="11">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="V44" s="11">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="V44" s="11">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
       <c r="X44" s="12">
-        <f t="shared" si="4"/>
-        <v>1.2642754365190653E-3</v>
+        <f t="shared" si="17"/>
+        <v>-0.70283208449578005</v>
       </c>
       <c r="Y44" s="12">
-        <f t="shared" si="8"/>
-        <v>1.2884498404129507E-3</v>
+        <f t="shared" si="18"/>
+        <v>-0.66290589051653548</v>
       </c>
       <c r="Z44" s="12">
-        <f t="shared" si="9"/>
-        <v>9.6441839609884283E-6</v>
+        <f t="shared" si="19"/>
+        <v>1.2615214565768695E-2</v>
       </c>
     </row>
     <row r="45" spans="2:26" x14ac:dyDescent="0.2">
       <c r="F45" s="15">
-        <f t="shared" si="16"/>
-        <v>20</v>
+        <f t="shared" si="15"/>
+        <v>19</v>
       </c>
       <c r="G45" s="30">
         <f t="shared" si="10"/>
-        <v>119.99979999999994</v>
+        <v>117.10000000000011</v>
       </c>
       <c r="H45" s="31">
+        <f t="shared" si="16"/>
+        <v>0.22880370091609967</v>
+      </c>
+      <c r="I45" s="17">
+        <v>0</v>
+      </c>
+      <c r="J45" s="16">
+        <v>0</v>
+      </c>
+      <c r="K45" s="15">
         <f t="shared" si="11"/>
-        <v>0.50049472860628974</v>
-      </c>
-      <c r="I45" s="17">
-        <v>0</v>
-      </c>
-      <c r="J45" s="16">
-        <v>0</v>
-      </c>
-      <c r="K45" s="15">
+        <v>0</v>
+      </c>
+      <c r="L45" s="15">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="L45" s="15">
-        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="M45" s="14">
@@ -3364,24 +3365,76 @@
         <v>0</v>
       </c>
       <c r="U45" s="11">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="V45" s="11">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="V45" s="11">
+      <c r="X45" s="12">
+        <f t="shared" si="17"/>
+        <v>-0.74279235973735469</v>
+      </c>
+      <c r="Y45" s="12">
+        <f t="shared" si="18"/>
+        <v>-0.70283208449578005</v>
+      </c>
+      <c r="Z45" s="12">
+        <f t="shared" si="19"/>
+        <v>1.2276498958544851E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="F46" s="15">
         <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="X45" s="12">
-        <f t="shared" si="4"/>
-        <v>1.2401010306428498E-3</v>
-      </c>
-      <c r="Y45" s="12">
-        <f t="shared" si="8"/>
-        <v>1.2642754365190653E-3</v>
-      </c>
-      <c r="Z45" s="12">
-        <f t="shared" si="9"/>
-        <v>9.6441850463424572E-6</v>
+        <v>20</v>
+      </c>
+      <c r="G46" s="30">
+        <f t="shared" si="10"/>
+        <v>117.00000000000011</v>
+      </c>
+      <c r="H46" s="31">
+        <f t="shared" si="16"/>
+        <v>0.21687616764146853</v>
+      </c>
+      <c r="I46" s="17">
+        <v>0</v>
+      </c>
+      <c r="J46" s="16">
+        <v>0</v>
+      </c>
+      <c r="K46" s="15">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="L46" s="15">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="M46" s="14">
+        <f>L46*$G$25*RiskFactors!$C$25</f>
+        <v>0</v>
+      </c>
+      <c r="U46" s="11">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="V46" s="11">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="X46" s="12">
+        <f t="shared" si="17"/>
+        <v>-0.78278677447496248</v>
+      </c>
+      <c r="Y46" s="12">
+        <f t="shared" si="18"/>
+        <v>-0.74279235973735469</v>
+      </c>
+      <c r="Z46" s="12">
+        <f t="shared" si="19"/>
+        <v>1.1927533274631141E-2</v>
       </c>
     </row>
     <row r="51" spans="6:13" x14ac:dyDescent="0.2">
@@ -3411,22 +3464,22 @@
     </row>
     <row r="53" spans="6:13" x14ac:dyDescent="0.2">
       <c r="F53" s="15">
-        <f t="shared" ref="F53:F72" si="17">1+F54</f>
+        <f t="shared" ref="F53:F72" si="20">1+F54</f>
         <v>21</v>
       </c>
       <c r="G53" s="30">
-        <f t="shared" ref="G53:G73" si="18">G54+$C$14</f>
-        <v>120.00021000000007</v>
+        <f t="shared" ref="G53:G73" si="21">G54+$C$15</f>
+        <v>123.09999999999988</v>
       </c>
     </row>
     <row r="54" spans="6:13" x14ac:dyDescent="0.2">
       <c r="F54" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>20</v>
       </c>
       <c r="G54" s="30">
-        <f t="shared" si="18"/>
-        <v>120.00020000000006</v>
+        <f t="shared" si="21"/>
+        <v>122.99999999999989</v>
       </c>
       <c r="I54" s="17">
         <v>0</v>
@@ -3442,18 +3495,18 @@
     </row>
     <row r="55" spans="6:13" x14ac:dyDescent="0.2">
       <c r="F55" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>19</v>
       </c>
       <c r="G55" s="30">
-        <f t="shared" si="18"/>
-        <v>120.00019000000006</v>
+        <f t="shared" si="21"/>
+        <v>122.89999999999989</v>
       </c>
       <c r="I55" s="17">
         <v>0</v>
       </c>
       <c r="L55" s="15">
-        <f t="shared" ref="L55:L94" si="19">I55</f>
+        <f t="shared" ref="L55:L74" si="22">I55</f>
         <v>0</v>
       </c>
       <c r="M55" s="14">
@@ -3463,18 +3516,18 @@
     </row>
     <row r="56" spans="6:13" x14ac:dyDescent="0.2">
       <c r="F56" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>18</v>
       </c>
       <c r="G56" s="30">
-        <f t="shared" si="18"/>
-        <v>120.00018000000006</v>
+        <f t="shared" si="21"/>
+        <v>122.7999999999999</v>
       </c>
       <c r="I56" s="17">
         <v>0</v>
       </c>
       <c r="L56" s="15">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="M56" s="14">
@@ -3484,18 +3537,18 @@
     </row>
     <row r="57" spans="6:13" x14ac:dyDescent="0.2">
       <c r="F57" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>17</v>
       </c>
       <c r="G57" s="30">
-        <f t="shared" si="18"/>
-        <v>120.00017000000005</v>
+        <f t="shared" si="21"/>
+        <v>122.6999999999999</v>
       </c>
       <c r="I57" s="17">
         <v>0</v>
       </c>
       <c r="L57" s="15">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="M57" s="14">
@@ -3505,18 +3558,18 @@
     </row>
     <row r="58" spans="6:13" x14ac:dyDescent="0.2">
       <c r="F58" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>16</v>
       </c>
       <c r="G58" s="30">
-        <f t="shared" si="18"/>
-        <v>120.00016000000005</v>
+        <f t="shared" si="21"/>
+        <v>122.59999999999991</v>
       </c>
       <c r="I58" s="17">
         <v>0</v>
       </c>
       <c r="L58" s="15">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="M58" s="14">
@@ -3526,18 +3579,18 @@
     </row>
     <row r="59" spans="6:13" x14ac:dyDescent="0.2">
       <c r="F59" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>15</v>
       </c>
       <c r="G59" s="30">
-        <f t="shared" si="18"/>
-        <v>120.00015000000005</v>
+        <f t="shared" si="21"/>
+        <v>122.49999999999991</v>
       </c>
       <c r="I59" s="17">
         <v>0</v>
       </c>
       <c r="L59" s="15">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="M59" s="14">
@@ -3547,18 +3600,18 @@
     </row>
     <row r="60" spans="6:13" x14ac:dyDescent="0.2">
       <c r="F60" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>14</v>
       </c>
       <c r="G60" s="30">
-        <f t="shared" si="18"/>
-        <v>120.00014000000004</v>
+        <f t="shared" si="21"/>
+        <v>122.39999999999992</v>
       </c>
       <c r="I60" s="17">
         <v>0</v>
       </c>
       <c r="L60" s="15">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="M60" s="14">
@@ -3568,18 +3621,18 @@
     </row>
     <row r="61" spans="6:13" x14ac:dyDescent="0.2">
       <c r="F61" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>13</v>
       </c>
       <c r="G61" s="30">
-        <f t="shared" si="18"/>
-        <v>120.00013000000004</v>
+        <f t="shared" si="21"/>
+        <v>122.29999999999993</v>
       </c>
       <c r="I61" s="17">
         <v>0</v>
       </c>
       <c r="L61" s="15">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="M61" s="14">
@@ -3589,18 +3642,18 @@
     </row>
     <row r="62" spans="6:13" x14ac:dyDescent="0.2">
       <c r="F62" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>12</v>
       </c>
       <c r="G62" s="30">
-        <f t="shared" si="18"/>
-        <v>120.00012000000004</v>
+        <f t="shared" si="21"/>
+        <v>122.19999999999993</v>
       </c>
       <c r="I62" s="17">
         <v>0</v>
       </c>
       <c r="L62" s="15">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="M62" s="14">
@@ -3610,18 +3663,18 @@
     </row>
     <row r="63" spans="6:13" x14ac:dyDescent="0.2">
       <c r="F63" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>11</v>
       </c>
       <c r="G63" s="30">
-        <f t="shared" si="18"/>
-        <v>120.00011000000003</v>
+        <f t="shared" si="21"/>
+        <v>122.09999999999994</v>
       </c>
       <c r="I63" s="17">
         <v>0</v>
       </c>
       <c r="L63" s="15">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="M63" s="14">
@@ -3631,39 +3684,39 @@
     </row>
     <row r="64" spans="6:13" x14ac:dyDescent="0.2">
       <c r="F64" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>10</v>
       </c>
       <c r="G64" s="30">
-        <f t="shared" si="18"/>
-        <v>120.00010000000003</v>
+        <f t="shared" si="21"/>
+        <v>121.99999999999994</v>
       </c>
       <c r="I64" s="17">
         <v>167</v>
       </c>
       <c r="L64" s="15">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>167</v>
       </c>
       <c r="M64" s="14">
         <f>L64*$G$25*RiskFactors!$C$24</f>
-        <v>233.84628325664463</v>
+        <v>1502.3300541970177</v>
       </c>
     </row>
     <row r="65" spans="5:13" x14ac:dyDescent="0.2">
       <c r="F65" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>9</v>
       </c>
       <c r="G65" s="30">
-        <f t="shared" si="18"/>
-        <v>120.00009000000003</v>
+        <f t="shared" si="21"/>
+        <v>121.89999999999995</v>
       </c>
       <c r="I65" s="17">
         <v>0</v>
       </c>
       <c r="L65" s="15">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="M65" s="14">
@@ -3673,18 +3726,18 @@
     </row>
     <row r="66" spans="5:13" x14ac:dyDescent="0.2">
       <c r="F66" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>8</v>
       </c>
       <c r="G66" s="30">
-        <f t="shared" si="18"/>
-        <v>120.00008000000003</v>
+        <f t="shared" si="21"/>
+        <v>121.79999999999995</v>
       </c>
       <c r="I66" s="17">
         <v>0</v>
       </c>
       <c r="L66" s="15">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="M66" s="14">
@@ -3694,18 +3747,18 @@
     </row>
     <row r="67" spans="5:13" x14ac:dyDescent="0.2">
       <c r="F67" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>7</v>
       </c>
       <c r="G67" s="30">
-        <f t="shared" si="18"/>
-        <v>120.00007000000002</v>
+        <f t="shared" si="21"/>
+        <v>121.69999999999996</v>
       </c>
       <c r="I67" s="17">
         <v>0</v>
       </c>
       <c r="L67" s="15">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="M67" s="14">
@@ -3715,18 +3768,18 @@
     </row>
     <row r="68" spans="5:13" x14ac:dyDescent="0.2">
       <c r="F68" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>6</v>
       </c>
       <c r="G68" s="30">
-        <f t="shared" si="18"/>
-        <v>120.00006000000002</v>
+        <f t="shared" si="21"/>
+        <v>121.59999999999997</v>
       </c>
       <c r="I68" s="17">
         <v>0</v>
       </c>
       <c r="L68" s="15">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="M68" s="14">
@@ -3736,18 +3789,18 @@
     </row>
     <row r="69" spans="5:13" x14ac:dyDescent="0.2">
       <c r="F69" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>5</v>
       </c>
       <c r="G69" s="30">
-        <f t="shared" si="18"/>
-        <v>120.00005000000002</v>
+        <f t="shared" si="21"/>
+        <v>121.49999999999997</v>
       </c>
       <c r="I69" s="17">
         <v>0</v>
       </c>
       <c r="L69" s="15">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="M69" s="14">
@@ -3757,18 +3810,18 @@
     </row>
     <row r="70" spans="5:13" x14ac:dyDescent="0.2">
       <c r="F70" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>4</v>
       </c>
       <c r="G70" s="30">
-        <f t="shared" si="18"/>
-        <v>120.00004000000001</v>
+        <f t="shared" si="21"/>
+        <v>121.39999999999998</v>
       </c>
       <c r="I70" s="17">
         <v>0</v>
       </c>
       <c r="L70" s="15">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="M70" s="14">
@@ -3778,18 +3831,18 @@
     </row>
     <row r="71" spans="5:13" x14ac:dyDescent="0.2">
       <c r="F71" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>3</v>
       </c>
       <c r="G71" s="30">
-        <f t="shared" si="18"/>
-        <v>120.00003000000001</v>
+        <f t="shared" si="21"/>
+        <v>121.29999999999998</v>
       </c>
       <c r="I71" s="17">
         <v>0</v>
       </c>
       <c r="L71" s="15">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="M71" s="14">
@@ -3799,18 +3852,18 @@
     </row>
     <row r="72" spans="5:13" x14ac:dyDescent="0.2">
       <c r="F72" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>2</v>
       </c>
       <c r="G72" s="30">
-        <f t="shared" si="18"/>
-        <v>120.00002000000001</v>
+        <f t="shared" si="21"/>
+        <v>121.19999999999999</v>
       </c>
       <c r="I72" s="17">
         <v>0</v>
       </c>
       <c r="L72" s="15">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="M72" s="14">
@@ -3823,120 +3876,100 @@
         <v>1</v>
       </c>
       <c r="G73" s="30">
-        <f t="shared" si="18"/>
-        <v>120.00001</v>
+        <f t="shared" si="21"/>
+        <v>121.1</v>
       </c>
       <c r="I73" s="17">
         <v>1</v>
       </c>
       <c r="L73" s="15">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>1</v>
       </c>
       <c r="M73" s="14">
         <f>L73*$G$25*RiskFactors!$C$24</f>
-        <v>1.400277145249369</v>
+        <v>8.9959883484851364</v>
       </c>
     </row>
     <row r="74" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E74" s="24" t="s">
-        <v>36</v>
+        <v>72</v>
       </c>
       <c r="F74" s="5">
         <v>0</v>
       </c>
       <c r="G74" s="29">
         <f>$C$13</f>
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="I74" s="5" t="s">
         <v>67</v>
       </c>
       <c r="L74" s="24" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>Another party LO volume</v>
       </c>
       <c r="M74" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="75" spans="5:13" x14ac:dyDescent="0.2">
-      <c r="F75" s="15">
+    <row r="76" spans="5:13" x14ac:dyDescent="0.2">
+      <c r="E76" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="F76" s="5">
+        <v>0</v>
+      </c>
+      <c r="G76" s="29">
+        <f>$C$14</f>
+        <v>119</v>
+      </c>
+      <c r="I76" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="L76" s="24" t="str">
+        <f t="shared" ref="L76" si="23">I76</f>
+        <v>Another party LO volume</v>
+      </c>
+      <c r="M76" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="77" spans="5:13" x14ac:dyDescent="0.2">
+      <c r="F77" s="15">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="G75" s="30">
-        <f t="shared" ref="G75:G94" si="20">G74-$C$14</f>
-        <v>119.99999</v>
-      </c>
-      <c r="I75" s="17">
+      <c r="G77" s="30">
+        <f t="shared" ref="G77:G96" si="24">G76-$C$15</f>
+        <v>118.9</v>
+      </c>
+      <c r="I77" s="17">
         <v>1</v>
       </c>
-      <c r="L75" s="15">
-        <f t="shared" si="19"/>
+      <c r="L77" s="15">
+        <f t="shared" ref="L77:L96" si="25">I77</f>
         <v>1</v>
-      </c>
-      <c r="M75" s="14">
-        <f>L75*$G$25*RiskFactors!$C$25</f>
-        <v>1.3854397691884524</v>
-      </c>
-    </row>
-    <row r="76" spans="5:13" x14ac:dyDescent="0.2">
-      <c r="F76" s="15">
-        <f t="shared" ref="F76:F94" si="21">1+F75</f>
-        <v>2</v>
-      </c>
-      <c r="G76" s="30">
-        <f t="shared" si="20"/>
-        <v>119.99997999999999</v>
-      </c>
-      <c r="I76" s="17">
-        <v>0</v>
-      </c>
-      <c r="L76" s="15">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="M76" s="14">
-        <f>L76*$G$25*RiskFactors!$C$25</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="5:13" x14ac:dyDescent="0.2">
-      <c r="F77" s="15">
-        <f t="shared" si="21"/>
-        <v>3</v>
-      </c>
-      <c r="G77" s="30">
-        <f t="shared" si="20"/>
-        <v>119.99996999999999</v>
-      </c>
-      <c r="I77" s="17">
-        <v>0</v>
-      </c>
-      <c r="L77" s="15">
-        <f t="shared" si="19"/>
-        <v>0</v>
       </c>
       <c r="M77" s="14">
         <f>L77*$G$25*RiskFactors!$C$25</f>
-        <v>0</v>
+        <v>8.4213514885393312</v>
       </c>
     </row>
     <row r="78" spans="5:13" x14ac:dyDescent="0.2">
       <c r="F78" s="15">
-        <f t="shared" si="21"/>
-        <v>4</v>
+        <f t="shared" ref="F78:F96" si="26">1+F77</f>
+        <v>2</v>
       </c>
       <c r="G78" s="30">
-        <f t="shared" si="20"/>
-        <v>119.99995999999999</v>
+        <f t="shared" si="24"/>
+        <v>118.80000000000001</v>
       </c>
       <c r="I78" s="17">
         <v>0</v>
       </c>
       <c r="L78" s="15">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="M78" s="14">
@@ -3946,18 +3979,18 @@
     </row>
     <row r="79" spans="5:13" x14ac:dyDescent="0.2">
       <c r="F79" s="15">
-        <f t="shared" si="21"/>
-        <v>5</v>
+        <f t="shared" si="26"/>
+        <v>3</v>
       </c>
       <c r="G79" s="30">
-        <f t="shared" si="20"/>
-        <v>119.99994999999998</v>
+        <f t="shared" si="24"/>
+        <v>118.70000000000002</v>
       </c>
       <c r="I79" s="17">
         <v>0</v>
       </c>
       <c r="L79" s="15">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="M79" s="14">
@@ -3967,18 +4000,18 @@
     </row>
     <row r="80" spans="5:13" x14ac:dyDescent="0.2">
       <c r="F80" s="15">
-        <f t="shared" si="21"/>
-        <v>6</v>
+        <f t="shared" si="26"/>
+        <v>4</v>
       </c>
       <c r="G80" s="30">
-        <f t="shared" si="20"/>
-        <v>119.99993999999998</v>
+        <f t="shared" si="24"/>
+        <v>118.60000000000002</v>
       </c>
       <c r="I80" s="17">
         <v>0</v>
       </c>
       <c r="L80" s="15">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="M80" s="14">
@@ -3988,18 +4021,18 @@
     </row>
     <row r="81" spans="6:13" x14ac:dyDescent="0.2">
       <c r="F81" s="15">
-        <f t="shared" si="21"/>
-        <v>7</v>
+        <f t="shared" si="26"/>
+        <v>5</v>
       </c>
       <c r="G81" s="30">
-        <f t="shared" si="20"/>
-        <v>119.99992999999998</v>
+        <f t="shared" si="24"/>
+        <v>118.50000000000003</v>
       </c>
       <c r="I81" s="17">
         <v>0</v>
       </c>
       <c r="L81" s="15">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="M81" s="14">
@@ -4009,18 +4042,18 @@
     </row>
     <row r="82" spans="6:13" x14ac:dyDescent="0.2">
       <c r="F82" s="15">
-        <f t="shared" si="21"/>
-        <v>8</v>
+        <f t="shared" si="26"/>
+        <v>6</v>
       </c>
       <c r="G82" s="30">
-        <f t="shared" si="20"/>
-        <v>119.99991999999997</v>
+        <f t="shared" si="24"/>
+        <v>118.40000000000003</v>
       </c>
       <c r="I82" s="17">
         <v>0</v>
       </c>
       <c r="L82" s="15">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="M82" s="14">
@@ -4030,18 +4063,18 @@
     </row>
     <row r="83" spans="6:13" x14ac:dyDescent="0.2">
       <c r="F83" s="15">
-        <f t="shared" si="21"/>
-        <v>9</v>
+        <f t="shared" si="26"/>
+        <v>7</v>
       </c>
       <c r="G83" s="30">
-        <f t="shared" si="20"/>
-        <v>119.99990999999997</v>
+        <f t="shared" si="24"/>
+        <v>118.30000000000004</v>
       </c>
       <c r="I83" s="17">
         <v>0</v>
       </c>
       <c r="L83" s="15">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="M83" s="14">
@@ -4051,39 +4084,39 @@
     </row>
     <row r="84" spans="6:13" x14ac:dyDescent="0.2">
       <c r="F84" s="15">
-        <f t="shared" si="21"/>
-        <v>10</v>
+        <f t="shared" si="26"/>
+        <v>8</v>
       </c>
       <c r="G84" s="30">
-        <f t="shared" si="20"/>
-        <v>119.99989999999997</v>
+        <f t="shared" si="24"/>
+        <v>118.20000000000005</v>
       </c>
       <c r="I84" s="17">
-        <v>167</v>
+        <v>0</v>
       </c>
       <c r="L84" s="15">
-        <f t="shared" si="19"/>
-        <v>167</v>
+        <f t="shared" si="25"/>
+        <v>0</v>
       </c>
       <c r="M84" s="14">
         <f>L84*$G$25*RiskFactors!$C$25</f>
-        <v>231.36844145447154</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="6:13" x14ac:dyDescent="0.2">
       <c r="F85" s="15">
-        <f t="shared" si="21"/>
-        <v>11</v>
+        <f t="shared" si="26"/>
+        <v>9</v>
       </c>
       <c r="G85" s="30">
-        <f t="shared" si="20"/>
-        <v>119.99988999999997</v>
+        <f t="shared" si="24"/>
+        <v>118.10000000000005</v>
       </c>
       <c r="I85" s="17">
         <v>0</v>
       </c>
       <c r="L85" s="15">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="M85" s="14">
@@ -4093,39 +4126,39 @@
     </row>
     <row r="86" spans="6:13" x14ac:dyDescent="0.2">
       <c r="F86" s="15">
-        <f t="shared" si="21"/>
-        <v>12</v>
+        <f t="shared" si="26"/>
+        <v>10</v>
       </c>
       <c r="G86" s="30">
-        <f t="shared" si="20"/>
-        <v>119.99987999999996</v>
+        <f t="shared" si="24"/>
+        <v>118.00000000000006</v>
       </c>
       <c r="I86" s="17">
-        <v>0</v>
+        <v>167</v>
       </c>
       <c r="L86" s="15">
-        <f t="shared" si="19"/>
-        <v>0</v>
+        <f t="shared" si="25"/>
+        <v>167</v>
       </c>
       <c r="M86" s="14">
         <f>L86*$G$25*RiskFactors!$C$25</f>
-        <v>0</v>
+        <v>1406.3656985860682</v>
       </c>
     </row>
     <row r="87" spans="6:13" x14ac:dyDescent="0.2">
       <c r="F87" s="15">
-        <f t="shared" si="21"/>
-        <v>13</v>
+        <f t="shared" si="26"/>
+        <v>11</v>
       </c>
       <c r="G87" s="30">
-        <f t="shared" si="20"/>
-        <v>119.99986999999996</v>
+        <f t="shared" si="24"/>
+        <v>117.90000000000006</v>
       </c>
       <c r="I87" s="17">
         <v>0</v>
       </c>
       <c r="L87" s="15">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="M87" s="14">
@@ -4135,18 +4168,18 @@
     </row>
     <row r="88" spans="6:13" x14ac:dyDescent="0.2">
       <c r="F88" s="15">
-        <f t="shared" si="21"/>
-        <v>14</v>
+        <f t="shared" si="26"/>
+        <v>12</v>
       </c>
       <c r="G88" s="30">
-        <f t="shared" si="20"/>
-        <v>119.99985999999996</v>
+        <f t="shared" si="24"/>
+        <v>117.80000000000007</v>
       </c>
       <c r="I88" s="17">
         <v>0</v>
       </c>
       <c r="L88" s="15">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="M88" s="14">
@@ -4156,18 +4189,18 @@
     </row>
     <row r="89" spans="6:13" x14ac:dyDescent="0.2">
       <c r="F89" s="15">
-        <f t="shared" si="21"/>
-        <v>15</v>
+        <f t="shared" si="26"/>
+        <v>13</v>
       </c>
       <c r="G89" s="30">
-        <f t="shared" si="20"/>
-        <v>119.99984999999995</v>
+        <f t="shared" si="24"/>
+        <v>117.70000000000007</v>
       </c>
       <c r="I89" s="17">
         <v>0</v>
       </c>
       <c r="L89" s="15">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="M89" s="14">
@@ -4177,18 +4210,18 @@
     </row>
     <row r="90" spans="6:13" x14ac:dyDescent="0.2">
       <c r="F90" s="15">
-        <f t="shared" si="21"/>
-        <v>16</v>
+        <f t="shared" si="26"/>
+        <v>14</v>
       </c>
       <c r="G90" s="30">
-        <f t="shared" si="20"/>
-        <v>119.99983999999995</v>
+        <f t="shared" si="24"/>
+        <v>117.60000000000008</v>
       </c>
       <c r="I90" s="17">
         <v>0</v>
       </c>
       <c r="L90" s="15">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="M90" s="14">
@@ -4198,18 +4231,18 @@
     </row>
     <row r="91" spans="6:13" x14ac:dyDescent="0.2">
       <c r="F91" s="15">
-        <f t="shared" si="21"/>
-        <v>17</v>
+        <f t="shared" si="26"/>
+        <v>15</v>
       </c>
       <c r="G91" s="30">
-        <f t="shared" si="20"/>
-        <v>119.99982999999995</v>
+        <f t="shared" si="24"/>
+        <v>117.50000000000009</v>
       </c>
       <c r="I91" s="17">
         <v>0</v>
       </c>
       <c r="L91" s="15">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="M91" s="14">
@@ -4219,18 +4252,18 @@
     </row>
     <row r="92" spans="6:13" x14ac:dyDescent="0.2">
       <c r="F92" s="15">
-        <f t="shared" si="21"/>
-        <v>18</v>
+        <f t="shared" si="26"/>
+        <v>16</v>
       </c>
       <c r="G92" s="30">
-        <f t="shared" si="20"/>
-        <v>119.99981999999994</v>
+        <f t="shared" si="24"/>
+        <v>117.40000000000009</v>
       </c>
       <c r="I92" s="17">
         <v>0</v>
       </c>
       <c r="L92" s="15">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="M92" s="14">
@@ -4240,18 +4273,18 @@
     </row>
     <row r="93" spans="6:13" x14ac:dyDescent="0.2">
       <c r="F93" s="15">
-        <f t="shared" si="21"/>
-        <v>19</v>
+        <f t="shared" si="26"/>
+        <v>17</v>
       </c>
       <c r="G93" s="30">
-        <f t="shared" si="20"/>
-        <v>119.99980999999994</v>
+        <f t="shared" si="24"/>
+        <v>117.3000000000001</v>
       </c>
       <c r="I93" s="17">
         <v>0</v>
       </c>
       <c r="L93" s="15">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="M93" s="14">
@@ -4261,22 +4294,64 @@
     </row>
     <row r="94" spans="6:13" x14ac:dyDescent="0.2">
       <c r="F94" s="15">
-        <f t="shared" si="21"/>
-        <v>20</v>
+        <f t="shared" si="26"/>
+        <v>18</v>
       </c>
       <c r="G94" s="30">
-        <f t="shared" si="20"/>
-        <v>119.99979999999994</v>
+        <f t="shared" si="24"/>
+        <v>117.2000000000001</v>
       </c>
       <c r="I94" s="17">
         <v>0</v>
       </c>
       <c r="L94" s="15">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="M94" s="14">
         <f>L94*$G$25*RiskFactors!$C$25</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="6:13" x14ac:dyDescent="0.2">
+      <c r="F95" s="15">
+        <f t="shared" si="26"/>
+        <v>19</v>
+      </c>
+      <c r="G95" s="30">
+        <f t="shared" si="24"/>
+        <v>117.10000000000011</v>
+      </c>
+      <c r="I95" s="17">
+        <v>0</v>
+      </c>
+      <c r="L95" s="15">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="M95" s="14">
+        <f>L95*$G$25*RiskFactors!$C$25</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="6:13" x14ac:dyDescent="0.2">
+      <c r="F96" s="15">
+        <f t="shared" si="26"/>
+        <v>20</v>
+      </c>
+      <c r="G96" s="30">
+        <f t="shared" si="24"/>
+        <v>117.00000000000011</v>
+      </c>
+      <c r="I96" s="17">
+        <v>0</v>
+      </c>
+      <c r="L96" s="15">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="M96" s="14">
+        <f>L96*$G$25*RiskFactors!$C$25</f>
         <v>0</v>
       </c>
     </row>
@@ -4302,22 +4377,22 @@
     </row>
     <row r="101" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F101" s="15">
-        <f t="shared" ref="F101:F120" si="22">1+F102</f>
+        <f t="shared" ref="F101:F120" si="27">1+F102</f>
         <v>21</v>
       </c>
       <c r="G101" s="30">
-        <f t="shared" ref="G101:G121" si="23">G102+$C$14</f>
-        <v>120.00021000000007</v>
+        <f t="shared" ref="G101:G121" si="28">G102+$C$15</f>
+        <v>123.09999999999988</v>
       </c>
     </row>
     <row r="102" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F102" s="15">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>20</v>
       </c>
       <c r="G102" s="30">
-        <f t="shared" si="23"/>
-        <v>120.00020000000006</v>
+        <f t="shared" si="28"/>
+        <v>122.99999999999989</v>
       </c>
       <c r="L102" s="15">
         <f>L54+L5</f>
@@ -4326,253 +4401,253 @@
     </row>
     <row r="103" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F103" s="15">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>19</v>
       </c>
       <c r="G103" s="30">
-        <f t="shared" si="23"/>
-        <v>120.00019000000006</v>
+        <f t="shared" si="28"/>
+        <v>122.89999999999989</v>
       </c>
       <c r="L103" s="15">
-        <f t="shared" ref="L103:L121" si="24">L55+L6</f>
+        <f t="shared" ref="L103:L121" si="29">L55+L6</f>
         <v>0</v>
       </c>
     </row>
     <row r="104" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F104" s="15">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>18</v>
       </c>
       <c r="G104" s="30">
-        <f t="shared" si="23"/>
-        <v>120.00018000000006</v>
+        <f t="shared" si="28"/>
+        <v>122.7999999999999</v>
       </c>
       <c r="L104" s="15">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
     </row>
     <row r="105" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F105" s="15">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>17</v>
       </c>
       <c r="G105" s="30">
-        <f t="shared" si="23"/>
-        <v>120.00017000000005</v>
+        <f t="shared" si="28"/>
+        <v>122.6999999999999</v>
       </c>
       <c r="L105" s="15">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
     </row>
     <row r="106" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F106" s="15">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>16</v>
       </c>
       <c r="G106" s="30">
-        <f t="shared" si="23"/>
-        <v>120.00016000000005</v>
+        <f t="shared" si="28"/>
+        <v>122.59999999999991</v>
       </c>
       <c r="L106" s="15">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
     </row>
     <row r="107" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F107" s="15">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>15</v>
       </c>
       <c r="G107" s="30">
-        <f t="shared" si="23"/>
-        <v>120.00015000000005</v>
+        <f t="shared" si="28"/>
+        <v>122.49999999999991</v>
       </c>
       <c r="L107" s="15">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
     </row>
     <row r="108" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F108" s="15">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>14</v>
       </c>
       <c r="G108" s="30">
-        <f t="shared" si="23"/>
-        <v>120.00014000000004</v>
+        <f t="shared" si="28"/>
+        <v>122.39999999999992</v>
       </c>
       <c r="L108" s="15">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
     </row>
     <row r="109" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F109" s="15">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>13</v>
       </c>
       <c r="G109" s="30">
-        <f t="shared" si="23"/>
-        <v>120.00013000000004</v>
+        <f t="shared" si="28"/>
+        <v>122.29999999999993</v>
       </c>
       <c r="L109" s="15">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
     </row>
     <row r="110" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F110" s="15">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>12</v>
       </c>
       <c r="G110" s="30">
-        <f t="shared" si="23"/>
-        <v>120.00012000000004</v>
+        <f t="shared" si="28"/>
+        <v>122.19999999999993</v>
       </c>
       <c r="L110" s="15">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
     </row>
     <row r="111" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F111" s="15">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>11</v>
       </c>
       <c r="G111" s="30">
-        <f t="shared" si="23"/>
-        <v>120.00011000000003</v>
+        <f t="shared" si="28"/>
+        <v>122.09999999999994</v>
       </c>
       <c r="L111" s="15">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
     </row>
     <row r="112" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F112" s="15">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>10</v>
       </c>
       <c r="G112" s="30">
-        <f t="shared" si="23"/>
-        <v>120.00010000000003</v>
+        <f t="shared" si="28"/>
+        <v>121.99999999999994</v>
       </c>
       <c r="L112" s="15">
-        <f t="shared" si="24"/>
-        <v>334</v>
+        <f t="shared" si="29"/>
+        <v>286</v>
       </c>
     </row>
     <row r="113" spans="5:12" x14ac:dyDescent="0.2">
       <c r="F113" s="15">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>9</v>
       </c>
       <c r="G113" s="30">
-        <f t="shared" si="23"/>
-        <v>120.00009000000003</v>
+        <f t="shared" si="28"/>
+        <v>121.89999999999995</v>
       </c>
       <c r="L113" s="15">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
     </row>
     <row r="114" spans="5:12" x14ac:dyDescent="0.2">
       <c r="F114" s="15">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>8</v>
       </c>
       <c r="G114" s="30">
-        <f t="shared" si="23"/>
-        <v>120.00008000000003</v>
+        <f t="shared" si="28"/>
+        <v>121.79999999999995</v>
       </c>
       <c r="L114" s="15">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
     </row>
     <row r="115" spans="5:12" x14ac:dyDescent="0.2">
       <c r="F115" s="15">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>7</v>
       </c>
       <c r="G115" s="30">
-        <f t="shared" si="23"/>
-        <v>120.00007000000002</v>
+        <f t="shared" si="28"/>
+        <v>121.69999999999996</v>
       </c>
       <c r="L115" s="15">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
     </row>
     <row r="116" spans="5:12" x14ac:dyDescent="0.2">
       <c r="F116" s="15">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>6</v>
       </c>
       <c r="G116" s="30">
-        <f t="shared" si="23"/>
-        <v>120.00006000000002</v>
+        <f t="shared" si="28"/>
+        <v>121.59999999999997</v>
       </c>
       <c r="L116" s="15">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
     </row>
     <row r="117" spans="5:12" x14ac:dyDescent="0.2">
       <c r="F117" s="15">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>5</v>
       </c>
       <c r="G117" s="30">
-        <f t="shared" si="23"/>
-        <v>120.00005000000002</v>
+        <f t="shared" si="28"/>
+        <v>121.49999999999997</v>
       </c>
       <c r="L117" s="15">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
     </row>
     <row r="118" spans="5:12" x14ac:dyDescent="0.2">
       <c r="F118" s="15">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>4</v>
       </c>
       <c r="G118" s="30">
-        <f t="shared" si="23"/>
-        <v>120.00004000000001</v>
+        <f t="shared" si="28"/>
+        <v>121.39999999999998</v>
       </c>
       <c r="L118" s="15">
-        <f t="shared" si="24"/>
-        <v>0</v>
+        <f t="shared" si="29"/>
+        <v>95</v>
       </c>
     </row>
     <row r="119" spans="5:12" x14ac:dyDescent="0.2">
       <c r="F119" s="15">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>3</v>
       </c>
       <c r="G119" s="30">
-        <f t="shared" si="23"/>
-        <v>120.00003000000001</v>
+        <f t="shared" si="28"/>
+        <v>121.29999999999998</v>
       </c>
       <c r="L119" s="15">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
     </row>
     <row r="120" spans="5:12" x14ac:dyDescent="0.2">
       <c r="F120" s="15">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>2</v>
       </c>
       <c r="G120" s="30">
-        <f t="shared" si="23"/>
-        <v>120.00002000000001</v>
+        <f t="shared" si="28"/>
+        <v>121.19999999999999</v>
       </c>
       <c r="L120" s="15">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
     </row>
@@ -4581,11 +4656,11 @@
         <v>1</v>
       </c>
       <c r="G121" s="30">
-        <f t="shared" si="23"/>
-        <v>120.00001</v>
+        <f t="shared" si="28"/>
+        <v>121.1</v>
       </c>
       <c r="L121" s="15">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>1</v>
       </c>
     </row>
@@ -4598,7 +4673,7 @@
       </c>
       <c r="G122" s="29">
         <f>$C$13</f>
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="H122" s="24"/>
       <c r="I122" s="24"/>
@@ -4614,277 +4689,277 @@
         <v>1</v>
       </c>
       <c r="G123" s="30">
-        <f t="shared" ref="G123:G142" si="25">G122-$C$14</f>
-        <v>119.99999</v>
+        <f t="shared" ref="G123:G142" si="30">G122-$C$15</f>
+        <v>120.9</v>
       </c>
       <c r="L123" s="15">
-        <f>L75+L26</f>
+        <f>L77+L27</f>
         <v>1</v>
       </c>
     </row>
     <row r="124" spans="5:12" x14ac:dyDescent="0.2">
       <c r="F124" s="15">
-        <f t="shared" ref="F124:F142" si="26">1+F123</f>
+        <f t="shared" ref="F124:F142" si="31">1+F123</f>
         <v>2</v>
       </c>
       <c r="G124" s="30">
-        <f t="shared" si="25"/>
-        <v>119.99997999999999</v>
+        <f t="shared" si="30"/>
+        <v>120.80000000000001</v>
       </c>
       <c r="L124" s="15">
-        <f t="shared" ref="L124:L142" si="27">L76+L27</f>
+        <f>L78+L28</f>
         <v>0</v>
       </c>
     </row>
     <row r="125" spans="5:12" x14ac:dyDescent="0.2">
       <c r="F125" s="15">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>3</v>
       </c>
       <c r="G125" s="30">
-        <f t="shared" si="25"/>
-        <v>119.99996999999999</v>
+        <f t="shared" si="30"/>
+        <v>120.70000000000002</v>
       </c>
       <c r="L125" s="15">
-        <f t="shared" si="27"/>
+        <f>L79+L29</f>
         <v>0</v>
       </c>
     </row>
     <row r="126" spans="5:12" x14ac:dyDescent="0.2">
       <c r="F126" s="15">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>4</v>
       </c>
       <c r="G126" s="30">
-        <f t="shared" si="25"/>
-        <v>119.99995999999999</v>
+        <f t="shared" si="30"/>
+        <v>120.60000000000002</v>
       </c>
       <c r="L126" s="15">
-        <f t="shared" si="27"/>
+        <f>L80+L30</f>
         <v>0</v>
       </c>
     </row>
     <row r="127" spans="5:12" x14ac:dyDescent="0.2">
       <c r="F127" s="15">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>5</v>
       </c>
       <c r="G127" s="30">
-        <f t="shared" si="25"/>
-        <v>119.99994999999998</v>
+        <f t="shared" si="30"/>
+        <v>120.50000000000003</v>
       </c>
       <c r="L127" s="15">
-        <f t="shared" si="27"/>
+        <f>L81+L31</f>
         <v>0</v>
       </c>
     </row>
     <row r="128" spans="5:12" x14ac:dyDescent="0.2">
       <c r="F128" s="15">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>6</v>
       </c>
       <c r="G128" s="30">
-        <f t="shared" si="25"/>
-        <v>119.99993999999998</v>
+        <f t="shared" si="30"/>
+        <v>120.40000000000003</v>
       </c>
       <c r="L128" s="15">
-        <f t="shared" si="27"/>
+        <f>L82+L32</f>
         <v>0</v>
       </c>
     </row>
     <row r="129" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F129" s="15">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>7</v>
       </c>
       <c r="G129" s="30">
-        <f t="shared" si="25"/>
-        <v>119.99992999999998</v>
+        <f t="shared" si="30"/>
+        <v>120.30000000000004</v>
       </c>
       <c r="L129" s="15">
-        <f t="shared" si="27"/>
+        <f>L83+L33</f>
         <v>0</v>
       </c>
     </row>
     <row r="130" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F130" s="15">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>8</v>
       </c>
       <c r="G130" s="30">
-        <f t="shared" si="25"/>
-        <v>119.99991999999997</v>
+        <f t="shared" si="30"/>
+        <v>120.20000000000005</v>
       </c>
       <c r="L130" s="15">
-        <f t="shared" si="27"/>
+        <f>L84+L34</f>
         <v>0</v>
       </c>
     </row>
     <row r="131" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F131" s="15">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>9</v>
       </c>
       <c r="G131" s="30">
-        <f t="shared" si="25"/>
-        <v>119.99990999999997</v>
+        <f t="shared" si="30"/>
+        <v>120.10000000000005</v>
       </c>
       <c r="L131" s="15">
-        <f t="shared" si="27"/>
+        <f>L85+L35</f>
         <v>0</v>
       </c>
     </row>
     <row r="132" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F132" s="15">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>10</v>
       </c>
       <c r="G132" s="30">
-        <f t="shared" si="25"/>
-        <v>119.99989999999997</v>
+        <f t="shared" si="30"/>
+        <v>120.00000000000006</v>
       </c>
       <c r="L132" s="15">
-        <f t="shared" si="27"/>
-        <v>334</v>
+        <f>L86+L36</f>
+        <v>409</v>
       </c>
     </row>
     <row r="133" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F133" s="15">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>11</v>
       </c>
       <c r="G133" s="30">
-        <f t="shared" si="25"/>
-        <v>119.99988999999997</v>
+        <f t="shared" si="30"/>
+        <v>119.90000000000006</v>
       </c>
       <c r="L133" s="15">
-        <f t="shared" si="27"/>
+        <f>L87+L37</f>
         <v>0</v>
       </c>
     </row>
     <row r="134" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F134" s="15">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>12</v>
       </c>
       <c r="G134" s="30">
-        <f t="shared" si="25"/>
-        <v>119.99987999999996</v>
+        <f t="shared" si="30"/>
+        <v>119.80000000000007</v>
       </c>
       <c r="L134" s="15">
-        <f t="shared" si="27"/>
+        <f>L88+L38</f>
         <v>0</v>
       </c>
     </row>
     <row r="135" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F135" s="15">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>13</v>
       </c>
       <c r="G135" s="30">
-        <f t="shared" si="25"/>
-        <v>119.99986999999996</v>
+        <f t="shared" si="30"/>
+        <v>119.70000000000007</v>
       </c>
       <c r="L135" s="15">
-        <f t="shared" si="27"/>
+        <f>L89+L39</f>
         <v>0</v>
       </c>
     </row>
     <row r="136" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F136" s="15">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>14</v>
       </c>
       <c r="G136" s="30">
-        <f t="shared" si="25"/>
-        <v>119.99985999999996</v>
+        <f t="shared" si="30"/>
+        <v>119.60000000000008</v>
       </c>
       <c r="L136" s="15">
-        <f t="shared" si="27"/>
+        <f>L90+L40</f>
         <v>0</v>
       </c>
     </row>
     <row r="137" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F137" s="15">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>15</v>
       </c>
       <c r="G137" s="30">
-        <f t="shared" si="25"/>
-        <v>119.99984999999995</v>
+        <f t="shared" si="30"/>
+        <v>119.50000000000009</v>
       </c>
       <c r="L137" s="15">
-        <f t="shared" si="27"/>
+        <f>L91+L41</f>
         <v>0</v>
       </c>
     </row>
     <row r="138" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F138" s="15">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>16</v>
       </c>
       <c r="G138" s="30">
-        <f t="shared" si="25"/>
-        <v>119.99983999999995</v>
+        <f t="shared" si="30"/>
+        <v>119.40000000000009</v>
       </c>
       <c r="L138" s="15">
-        <f t="shared" si="27"/>
+        <f>L92+L42</f>
         <v>0</v>
       </c>
     </row>
     <row r="139" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F139" s="15">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>17</v>
       </c>
       <c r="G139" s="30">
-        <f t="shared" si="25"/>
-        <v>119.99982999999995</v>
+        <f t="shared" si="30"/>
+        <v>119.3000000000001</v>
       </c>
       <c r="L139" s="15">
-        <f t="shared" si="27"/>
+        <f>L93+L43</f>
         <v>0</v>
       </c>
     </row>
     <row r="140" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F140" s="15">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>18</v>
       </c>
       <c r="G140" s="30">
-        <f t="shared" si="25"/>
-        <v>119.99981999999994</v>
+        <f t="shared" si="30"/>
+        <v>119.2000000000001</v>
       </c>
       <c r="L140" s="15">
-        <f t="shared" si="27"/>
+        <f>L94+L44</f>
         <v>0</v>
       </c>
     </row>
     <row r="141" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F141" s="15">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>19</v>
       </c>
       <c r="G141" s="30">
-        <f t="shared" si="25"/>
-        <v>119.99980999999994</v>
+        <f t="shared" si="30"/>
+        <v>119.10000000000011</v>
       </c>
       <c r="L141" s="15">
-        <f t="shared" si="27"/>
+        <f>L95+L45</f>
         <v>0</v>
       </c>
     </row>
     <row r="142" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F142" s="15">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>20</v>
       </c>
       <c r="G142" s="30">
-        <f t="shared" si="25"/>
-        <v>119.99979999999994</v>
+        <f t="shared" si="30"/>
+        <v>119.00000000000011</v>
       </c>
       <c r="L142" s="15">
-        <f t="shared" si="27"/>
+        <f>L96+L46</f>
         <v>0</v>
       </c>
     </row>
@@ -5649,7 +5724,7 @@
       </c>
       <c r="M15" s="14">
         <f>L15*$G$25*RiskFactors!$C$24</f>
-        <v>23.80473130649883</v>
+        <v>151.66802912470968</v>
       </c>
       <c r="U15" s="11">
         <f t="shared" si="2"/>
@@ -5708,7 +5783,7 @@
       </c>
       <c r="M16" s="14">
         <f>L16*$G$25*RiskFactors!$C$24</f>
-        <v>23.80473130649883</v>
+        <v>151.66802912470968</v>
       </c>
       <c r="U16" s="11">
         <f t="shared" si="2"/>
@@ -5760,7 +5835,7 @@
       </c>
       <c r="M17" s="14">
         <f>L17*$G$25*RiskFactors!$C$24</f>
-        <v>23.80473130649883</v>
+        <v>151.66802912470968</v>
       </c>
       <c r="U17" s="11">
         <f t="shared" si="2"/>
@@ -5812,7 +5887,7 @@
       </c>
       <c r="M18" s="14">
         <f>L18*$G$25*RiskFactors!$C$24</f>
-        <v>23.80473130649883</v>
+        <v>151.66802912470968</v>
       </c>
       <c r="U18" s="11">
         <f t="shared" si="2"/>
@@ -5869,7 +5944,7 @@
       </c>
       <c r="M19" s="14">
         <f>L19*$G$25*RiskFactors!$C$24</f>
-        <v>23.80473130649883</v>
+        <v>151.66802912470968</v>
       </c>
       <c r="U19" s="11">
         <f t="shared" si="2"/>
@@ -5930,7 +6005,7 @@
       </c>
       <c r="M20" s="14">
         <f>L20*$G$25*RiskFactors!$C$24</f>
-        <v>23.80473130649883</v>
+        <v>151.66802912470968</v>
       </c>
       <c r="U20" s="11">
         <f t="shared" si="2"/>
@@ -5993,7 +6068,7 @@
       </c>
       <c r="M21" s="14">
         <f>L21*$G$25*RiskFactors!$C$24</f>
-        <v>23.80473130649883</v>
+        <v>151.66802912470968</v>
       </c>
       <c r="U21" s="11">
         <f t="shared" si="2"/>
@@ -6120,7 +6195,7 @@
       </c>
       <c r="M23" s="14">
         <f>L23*$G$25*RiskFactors!$C$24</f>
-        <v>70.013915607349503</v>
+        <v>446.08243860208728</v>
       </c>
       <c r="U23" s="11">
         <f t="shared" si="2"/>
@@ -6370,7 +6445,7 @@
       </c>
       <c r="M27" s="14">
         <f>L27*$G$25*RiskFactors!$C$25</f>
-        <v>26.323377550710276</v>
+        <v>158.68344954080581</v>
       </c>
       <c r="U27" s="11">
         <f t="shared" si="14"/>
@@ -6432,7 +6507,7 @@
       </c>
       <c r="M28" s="14">
         <f>L28*$G$25*RiskFactors!$C$25</f>
-        <v>26.323377550710276</v>
+        <v>158.68344954080581</v>
       </c>
       <c r="U28" s="11">
         <f t="shared" si="14"/>
@@ -6494,7 +6569,7 @@
       </c>
       <c r="M29" s="14">
         <f>L29*$G$25*RiskFactors!$C$25</f>
-        <v>26.323377550710276</v>
+        <v>158.68344954080581</v>
       </c>
       <c r="U29" s="11">
         <f t="shared" si="14"/>
@@ -6546,7 +6621,7 @@
       </c>
       <c r="M30" s="14">
         <f>L30*$G$25*RiskFactors!$C$25</f>
-        <v>26.323377550710276</v>
+        <v>158.68344954080581</v>
       </c>
       <c r="U30" s="11">
         <f t="shared" si="14"/>
@@ -6603,7 +6678,7 @@
       </c>
       <c r="M31" s="14">
         <f>L31*$G$25*RiskFactors!$C$25</f>
-        <v>26.323377550710276</v>
+        <v>158.68344954080581</v>
       </c>
       <c r="U31" s="11">
         <f t="shared" si="14"/>
@@ -6632,7 +6707,7 @@
       </c>
       <c r="C32" s="18">
         <f>SUM(M3:M33)</f>
-        <v>420.91067760781334</v>
+        <v>2618.5427892606954</v>
       </c>
       <c r="D32" s="15" t="str">
         <f>C15</f>
@@ -6666,7 +6741,7 @@
       </c>
       <c r="M32" s="14">
         <f>L32*$G$25*RiskFactors!$C$25</f>
-        <v>26.323377550710276</v>
+        <v>158.68344954080581</v>
       </c>
       <c r="U32" s="11">
         <f t="shared" si="14"/>
@@ -6695,7 +6770,7 @@
       </c>
       <c r="C33" s="18">
         <f>SUM(M26:M177)</f>
-        <v>1413.9435433587835</v>
+        <v>8728.7309614268088</v>
       </c>
       <c r="D33" s="15" t="str">
         <f>C15</f>
@@ -6729,7 +6804,7 @@
       </c>
       <c r="M33" s="14">
         <f>L33*$G$25*RiskFactors!$C$25</f>
-        <v>26.323377550710276</v>
+        <v>158.68344954080581</v>
       </c>
       <c r="U33" s="11">
         <f t="shared" si="14"/>
@@ -6781,7 +6856,7 @@
       </c>
       <c r="M34" s="14">
         <f>L34*$G$25*RiskFactors!$C$25</f>
-        <v>26.323377550710276</v>
+        <v>158.68344954080581</v>
       </c>
       <c r="U34" s="11">
         <f t="shared" si="14"/>
@@ -6838,7 +6913,7 @@
       </c>
       <c r="M35" s="14">
         <f>L35*$G$25*RiskFactors!$C$25</f>
-        <v>26.323377550710276</v>
+        <v>158.68344954080581</v>
       </c>
       <c r="U35" s="11">
         <f t="shared" si="14"/>
@@ -6867,7 +6942,7 @@
       </c>
       <c r="C36" s="14">
         <f>C20+SUM(C32:C33)</f>
-        <v>11834.854220966597</v>
+        <v>21347.273750687506</v>
       </c>
       <c r="D36" s="15" t="str">
         <f>C15</f>
@@ -7655,7 +7730,7 @@
       </c>
       <c r="M64" s="14">
         <f>L64*$G$25*RiskFactors!$C$24</f>
-        <v>233.84647812854735</v>
+        <v>1489.9153449309715</v>
       </c>
     </row>
     <row r="65" spans="5:13" x14ac:dyDescent="0.2">
@@ -7676,7 +7751,7 @@
       </c>
       <c r="M65" s="14">
         <f>L65*$G$25*RiskFactors!$C$24</f>
-        <v>70.013915607349503</v>
+        <v>446.08243860208728</v>
       </c>
     </row>
     <row r="66" spans="5:13" x14ac:dyDescent="0.2">
@@ -7697,7 +7772,7 @@
       </c>
       <c r="M66" s="14">
         <f>L66*$G$25*RiskFactors!$C$24</f>
-        <v>70.013915607349503</v>
+        <v>446.08243860208728</v>
       </c>
     </row>
     <row r="67" spans="5:13" x14ac:dyDescent="0.2">
@@ -7718,7 +7793,7 @@
       </c>
       <c r="M67" s="14">
         <f>L67*$G$25*RiskFactors!$C$24</f>
-        <v>70.013915607349503</v>
+        <v>446.08243860208728</v>
       </c>
     </row>
     <row r="68" spans="5:13" x14ac:dyDescent="0.2">
@@ -7739,7 +7814,7 @@
       </c>
       <c r="M68" s="14">
         <f>L68*$G$25*RiskFactors!$C$24</f>
-        <v>70.013915607349503</v>
+        <v>446.08243860208728</v>
       </c>
     </row>
     <row r="69" spans="5:13" x14ac:dyDescent="0.2">
@@ -7760,7 +7835,7 @@
       </c>
       <c r="M69" s="14">
         <f>L69*$G$25*RiskFactors!$C$24</f>
-        <v>70.013915607349503</v>
+        <v>446.08243860208728</v>
       </c>
     </row>
     <row r="70" spans="5:13" x14ac:dyDescent="0.2">
@@ -7781,7 +7856,7 @@
       </c>
       <c r="M70" s="14">
         <f>L70*$G$25*RiskFactors!$C$24</f>
-        <v>14.0027831214699</v>
+        <v>89.216487720417447</v>
       </c>
     </row>
     <row r="71" spans="5:13" x14ac:dyDescent="0.2">
@@ -7949,7 +8024,7 @@
       </c>
       <c r="M78" s="14">
         <f>L78*$G$25*RiskFactors!$C$25</f>
-        <v>1.3854409237215934</v>
+        <v>8.3517605021476751</v>
       </c>
     </row>
     <row r="79" spans="5:13" x14ac:dyDescent="0.2">
@@ -7970,7 +8045,7 @@
       </c>
       <c r="M79" s="14">
         <f>L79*$G$25*RiskFactors!$C$25</f>
-        <v>69.272046186079663</v>
+        <v>417.58802510738371</v>
       </c>
     </row>
     <row r="80" spans="5:13" x14ac:dyDescent="0.2">
@@ -7991,7 +8066,7 @@
       </c>
       <c r="M80" s="14">
         <f>L80*$G$25*RiskFactors!$C$25</f>
-        <v>69.272046186079663</v>
+        <v>417.58802510738371</v>
       </c>
     </row>
     <row r="81" spans="6:13" x14ac:dyDescent="0.2">
@@ -8012,7 +8087,7 @@
       </c>
       <c r="M81" s="14">
         <f>L81*$G$25*RiskFactors!$C$25</f>
-        <v>69.272046186079663</v>
+        <v>417.58802510738371</v>
       </c>
     </row>
     <row r="82" spans="6:13" x14ac:dyDescent="0.2">
@@ -8033,7 +8108,7 @@
       </c>
       <c r="M82" s="14">
         <f>L82*$G$25*RiskFactors!$C$25</f>
-        <v>69.272046186079663</v>
+        <v>417.58802510738371</v>
       </c>
     </row>
     <row r="83" spans="6:13" x14ac:dyDescent="0.2">
@@ -8054,7 +8129,7 @@
       </c>
       <c r="M83" s="14">
         <f>L83*$G$25*RiskFactors!$C$25</f>
-        <v>69.272046186079663</v>
+        <v>417.58802510738371</v>
       </c>
     </row>
     <row r="84" spans="6:13" x14ac:dyDescent="0.2">
@@ -8075,7 +8150,7 @@
       </c>
       <c r="M84" s="14">
         <f>L84*$G$25*RiskFactors!$C$25</f>
-        <v>231.36863426150609</v>
+        <v>1394.7440038586615</v>
       </c>
     </row>
     <row r="85" spans="6:13" x14ac:dyDescent="0.2">

</xml_diff>